<commit_message>
test 1 & 2 Writing!
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAA3BBC8-4917-4BC6-88A0-F3C05851D609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99E4F14-99B8-4B20-921D-5F423FD71AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -101,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,20 +106,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -186,7 +186,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,14 +204,17 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -666,28 +669,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:M16"/>
+  <dimension ref="C3:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="2.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" customWidth="1"/>
+    <col min="2" max="2" width="2.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -716,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:13">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C4" s="3">
         <v>45419</v>
       </c>
@@ -726,25 +729,25 @@
       <c r="E4" s="7">
         <v>26</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
       <c r="G4">
         <v>13</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>4.5</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
       <c r="K4" s="8">
         <f>(F4+H4+I4+J4)/4</f>
         <v>2.625</v>
       </c>
     </row>
-    <row r="5" spans="3:13">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C5" s="3">
         <v>45421</v>
       </c>
@@ -754,19 +757,19 @@
       <c r="E5" s="7">
         <v>22</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
       <c r="K5" s="8">
         <f>(F5+H5+I5+J5)/4</f>
         <v>1.375</v>
       </c>
     </row>
-    <row r="6" spans="3:13">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C6" s="3">
         <v>45428</v>
       </c>
@@ -776,27 +779,27 @@
       <c r="E6" s="7">
         <v>32</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
       <c r="G6">
         <v>20</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J6" s="12"/>
+      <c r="J6" s="10"/>
       <c r="K6" s="8">
         <f t="shared" ref="K6:K7" si="0">(F6+H6+I6+J6)/4</f>
         <v>3.4</v>
       </c>
     </row>
-    <row r="7" spans="3:13">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C7" s="3">
         <v>45429</v>
       </c>
@@ -806,27 +809,27 @@
       <c r="E7" s="7">
         <v>32</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="10">
         <v>4</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="10"/>
       <c r="K7" s="8">
         <f t="shared" si="0"/>
         <v>4.125</v>
       </c>
     </row>
-    <row r="8" spans="3:13">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C8" s="3">
         <v>45431</v>
       </c>
@@ -834,18 +837,18 @@
         <v>13</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12">
+      <c r="F8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10">
         <v>4.5</v>
       </c>
-      <c r="J8" s="12"/>
+      <c r="J8" s="10"/>
       <c r="K8" s="8">
         <f>(F8+H8+I8+J8)/4</f>
         <v>1.125</v>
       </c>
     </row>
-    <row r="9" spans="3:13">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C9" s="3">
         <v>45435</v>
       </c>
@@ -853,19 +856,22 @@
         <v>10</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="9"/>
       <c r="G9">
         <v>24</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="3:13">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="8">
+        <f t="shared" ref="K9:K10" si="1">(F9+H9+I9+J9)/4</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C10" s="3">
         <v>45436</v>
       </c>
@@ -875,71 +881,90 @@
       <c r="E10" s="7">
         <v>31</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
       <c r="G10">
         <v>20</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="8"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="8">
+        <f t="shared" si="1"/>
+        <v>3.125</v>
+      </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="3:13">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C11" s="3">
+        <v>45437</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="F11" s="9"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="3:13">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C12" s="3">
+        <v>45438</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="11"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="F12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="3:13">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E13" s="7"/>
-      <c r="F13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
+      <c r="F13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="3:13">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E14" s="7"/>
-      <c r="F14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="F14" s="9"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="3:13">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E15" s="7"/>
-      <c r="F15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="F15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="3:13">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E16" s="7"/>
-      <c r="F16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
+      <c r="F16" s="9"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
       <c r="K16" s="8"/>
     </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H19" s="11"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -955,28 +980,28 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:8">
-      <c r="D2" s="10" t="s">
+    <row r="2" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="4:8">
-      <c r="D3" s="9" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="4:8">
+    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
@@ -987,7 +1012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="4:8">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D5" s="5">
         <v>1</v>
       </c>
@@ -998,7 +1023,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="4:8">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D6" s="5">
         <v>2</v>
       </c>
@@ -1009,7 +1034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:8">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D7" s="5">
         <v>4</v>
       </c>
@@ -1020,7 +1045,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="4:8">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D8" s="5">
         <v>6</v>
       </c>
@@ -1031,7 +1056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="4:8">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D9" s="5">
         <v>8</v>
       </c>
@@ -1042,7 +1067,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="10" spans="4:8">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D10" s="5">
         <v>10</v>
       </c>
@@ -1053,7 +1078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="4:8">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D11" s="5">
         <v>13</v>
       </c>
@@ -1064,7 +1089,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="12" spans="4:8">
+    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D12" s="5">
         <v>15</v>
       </c>
@@ -1078,7 +1103,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="4:8">
+    <row r="13" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D13" s="5">
         <v>19</v>
       </c>
@@ -1089,7 +1114,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="14" spans="4:8">
+    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D14" s="5">
         <v>23</v>
       </c>
@@ -1100,7 +1125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="4:8">
+    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D15" s="5">
         <v>27</v>
       </c>
@@ -1111,7 +1136,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="16" spans="4:8">
+    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D16" s="5">
         <v>30</v>
       </c>
@@ -1122,7 +1147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D17" s="5">
         <v>33</v>
       </c>
@@ -1133,7 +1158,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="18" spans="4:6">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D18" s="5">
         <v>35</v>
       </c>
@@ -1144,7 +1169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="4:6">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D19" s="5">
         <v>37</v>
       </c>
@@ -1155,7 +1180,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D20" s="5">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Practiced IELTS 11 Test 2 Reading.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ABCA67-365B-4CBD-A119-02947FF96E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D96BD0-BA37-4B52-BD70-894EC271E9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>a Practice Test</t>
+  </si>
+  <si>
+    <t>IELTS11_Test3</t>
+  </si>
+  <si>
+    <t>IELTS11_Test4</t>
   </si>
 </sst>
 </file>
@@ -101,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +139,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -192,7 +204,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,9 +224,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:K16" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="C3:K16" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:K21" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="C3:K21" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date"/>
     <tableColumn id="2" xr3:uid="{DC71C96E-388E-4427-9265-6CF875C8C5D7}" name="Course"/>
@@ -675,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:M19"/>
+  <dimension ref="C3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,12 +987,21 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H14" s="10"/>
+      <c r="G14">
+        <v>28</v>
+      </c>
+      <c r="H14" s="10">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="8"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="9"/>
       <c r="H15" s="10"/>
@@ -986,6 +1010,9 @@
       <c r="K15" s="8"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="9"/>
       <c r="H16" s="10"/>
@@ -993,8 +1020,45 @@
       <c r="J16" s="10"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H19" s="11"/>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E17" s="7"/>
+      <c r="F17" s="11"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E18" s="7"/>
+      <c r="F18" s="11"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E19" s="7"/>
+      <c r="F19" s="11"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E20" s="7"/>
+      <c r="F20" s="11"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E21" s="7"/>
+      <c r="F21" s="11"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1021,17 +1085,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Practiced IELTS 11 Test 3 Listening
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D96BD0-BA37-4B52-BD70-894EC271E9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4D05C3-A75F-478C-8D2D-B731113528B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <dimension ref="C3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -994,16 +994,26 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="I14" s="10"/>
+      <c r="I14" s="10">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="J14" s="10"/>
       <c r="K14" s="8"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C15" s="3">
+        <v>45449</v>
+      </c>
       <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="7">
+        <v>34</v>
+      </c>
+      <c r="F15" s="9">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7.5</v>
+      </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>

</xml_diff>

<commit_message>
Practiced Cambridge 11 Test 3 Reading.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4D05C3-A75F-478C-8D2D-B731113528B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285AA927-C748-4A00-9CE9-822C67E4A83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,6 +236,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -335,8 +336,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:K21" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="C3:K21" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:K25" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="C3:K25" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date"/>
     <tableColumn id="2" xr3:uid="{DC71C96E-388E-4427-9265-6CF875C8C5D7}" name="Course"/>
@@ -690,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:M21"/>
+  <dimension ref="C3:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,10 +764,7 @@
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="8">
-        <f>(F4+H4+I4+J4)/4</f>
-        <v>2.625</v>
-      </c>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C5" s="3">
@@ -785,10 +783,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="8">
-        <f>(F5+H5+I5+J5)/4</f>
-        <v>1.375</v>
-      </c>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C6" s="3">
@@ -816,8 +811,8 @@
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="8">
-        <f t="shared" ref="K6:K7" si="0">(F6+H6+I6+J6)/4</f>
-        <v>3.4</v>
+        <f t="shared" ref="K6:K16" si="0">(F6+H6+I6+J6)/3</f>
+        <v>4.5333333333333332</v>
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.35">
@@ -847,7 +842,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="8">
         <f t="shared" si="0"/>
-        <v>4.125</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.35">
@@ -864,10 +859,7 @@
         <v>4.5</v>
       </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="8">
-        <f>(F8+H8+I8+J8)/4</f>
-        <v>1.125</v>
-      </c>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C9" s="3">
@@ -887,10 +879,7 @@
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="8">
-        <f t="shared" ref="K9:K10" si="1">(F9+H9+I9+J9)/4</f>
-        <v>1.5</v>
-      </c>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C10" s="3">
@@ -916,8 +905,7 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="8">
-        <f t="shared" si="1"/>
-        <v>3.125</v>
+        <v>6</v>
       </c>
       <c r="M10" s="8"/>
     </row>
@@ -998,7 +986,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J14" s="10"/>
-      <c r="K14" s="8"/>
+      <c r="K14" s="8">
+        <f t="shared" si="0"/>
+        <v>4.8666666666666663</v>
+      </c>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C15" s="3">
@@ -1014,10 +1005,21 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="G15">
+        <v>29</v>
+      </c>
+      <c r="H15" s="10">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
       <c r="J15" s="10"/>
-      <c r="K15" s="8"/>
+      <c r="K15" s="8">
+        <f t="shared" si="0"/>
+        <v>4.666666666666667</v>
+      </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
@@ -1028,7 +1030,10 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="8"/>
+      <c r="K16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E17" s="7"/>
@@ -1069,6 +1074,38 @@
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E22" s="7"/>
+      <c r="F22" s="11"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E23" s="7"/>
+      <c r="F23" s="11"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E24" s="7"/>
+      <c r="F24" s="11"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E25" s="7"/>
+      <c r="F25" s="11"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Practiced Cambridge 14 Test 4.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C1A6EA-A84C-4212-A85E-FE9B4CB504D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE75467-73A0-4A9B-B222-F13CEFF0C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>IELTS14_Test3</t>
+  </si>
+  <si>
+    <t>IELTS14_Test4</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <dimension ref="C3:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1201,14 +1204,37 @@
         <v>4.875</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C20" s="13"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="7"/>
+    <row r="20" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="13">
+        <v>45466</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="6">
+        <v>32</v>
+      </c>
+      <c r="F20" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>26</v>
+      </c>
+      <c r="H20" s="9">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6</v>
+      </c>
+      <c r="I20" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J20" s="12">
+        <v>3</v>
+      </c>
+      <c r="K20" s="7">
+        <f>(F20+H20+I20+J20)/4</f>
+        <v>4.2750000000000004</v>
+      </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.35">
       <c r="E21" s="6"/>

</xml_diff>

<commit_message>
Practiced Cambridge 17 Test 1.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAF04E2-AC70-4A85-AB33-F917E4E8F324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6298614D-1BC0-48D0-80DA-25F1E9603C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>Band_Score</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>IELTS11_Test2</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>IELTS14_Test4</t>
+  </si>
+  <si>
+    <t>IELTS17_Test1</t>
   </si>
 </sst>
 </file>
@@ -700,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:M25"/>
+  <dimension ref="C1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -721,6 +721,8 @@
     <col min="11" max="11" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="3:13" ht="6.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:13" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -773,11 +775,11 @@
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" ref="K4:K17" si="0">(F4+H4+I4+J4)/4</f>
-        <v>3.375</v>
+        <v>3.625</v>
       </c>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -797,11 +799,11 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="0"/>
-        <v>2.125</v>
+        <v>2.375</v>
       </c>
     </row>
     <row r="6" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -829,11 +831,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J6" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="0"/>
-        <v>4.1500000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="7" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -861,11 +863,11 @@
         <v>4</v>
       </c>
       <c r="J7" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="0"/>
-        <v>4.875</v>
+        <v>5.125</v>
       </c>
     </row>
     <row r="8" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -882,11 +884,11 @@
         <v>4.5</v>
       </c>
       <c r="J8" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="0"/>
-        <v>1.875</v>
+        <v>2.125</v>
       </c>
     </row>
     <row r="9" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -907,11 +909,11 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="10" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -937,11 +939,11 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="0"/>
-        <v>3.875</v>
+        <v>4.125</v>
       </c>
       <c r="M10" s="7"/>
     </row>
@@ -959,11 +961,11 @@
         <v>6</v>
       </c>
       <c r="J11" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -980,11 +982,11 @@
         <v>4</v>
       </c>
       <c r="J12" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="0"/>
-        <v>1.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -992,7 +994,7 @@
         <v>45443</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="8"/>
@@ -1004,20 +1006,15 @@
         <v>6</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="9">
-        <v>3</v>
-      </c>
-      <c r="K13" s="7">
-        <f t="shared" si="0"/>
-        <v>2.25</v>
-      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="13">
         <v>45447</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6">
         <v>30</v>
@@ -1037,11 +1034,11 @@
         <v>6.5</v>
       </c>
       <c r="J14" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="0"/>
-        <v>5.75</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1049,7 +1046,7 @@
         <v>45449</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="6">
         <v>34</v>
@@ -1069,11 +1066,11 @@
         <v>5.5</v>
       </c>
       <c r="J15" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="0"/>
-        <v>5.625</v>
+        <v>5.875</v>
       </c>
     </row>
     <row r="16" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1081,7 +1078,7 @@
         <v>45452</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="6">
         <v>30</v>
@@ -1101,11 +1098,11 @@
         <v>5</v>
       </c>
       <c r="J16" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="0"/>
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="17" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1113,7 +1110,7 @@
         <v>45454</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="6">
         <v>33</v>
@@ -1133,11 +1130,11 @@
         <v>6.5</v>
       </c>
       <c r="J17" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="18" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1145,7 +1142,7 @@
         <v>45456</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="6">
         <v>33</v>
@@ -1165,11 +1162,11 @@
         <v>6</v>
       </c>
       <c r="J18" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K18" s="7">
         <f>(F18+H18+I18+J18)/4</f>
-        <v>5.625</v>
+        <v>5.875</v>
       </c>
     </row>
     <row r="19" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1177,7 +1174,7 @@
         <v>45457</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="6">
         <v>29</v>
@@ -1197,11 +1194,11 @@
         <v>4</v>
       </c>
       <c r="J19" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K19" s="7">
         <f>(F19+H19+I19+J19)/4</f>
-        <v>4.875</v>
+        <v>5.125</v>
       </c>
     </row>
     <row r="20" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1209,7 +1206,7 @@
         <v>45466</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="6">
         <v>32</v>
@@ -1228,21 +1225,45 @@
       <c r="I20" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J20" s="12">
-        <v>3</v>
+      <c r="J20" s="9">
+        <v>4</v>
       </c>
       <c r="K20" s="7">
         <f>(F20+H20+I20+J20)/4</f>
-        <v>4.2750000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="E21" s="6"/>
-      <c r="F21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="7"/>
+        <v>4.5250000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C21" s="13">
+        <v>45469</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="6">
+        <v>34</v>
+      </c>
+      <c r="F21" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7.5</v>
+      </c>
+      <c r="G21">
+        <v>29</v>
+      </c>
+      <c r="H21" s="9">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
+      <c r="I21" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J21" s="9">
+        <v>4</v>
+      </c>
+      <c r="K21" s="7">
+        <f>(F21+H21+I21+J21)/4</f>
+        <v>4.7750000000000004</v>
+      </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.35">
       <c r="E22" s="6"/>
@@ -1287,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD14B10B-0F91-47FE-B9A4-F4B2E360BE18}">
-  <dimension ref="D2:H20"/>
+  <dimension ref="D2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1300,21 +1321,21 @@
     <col min="6" max="6" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D3" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1325,7 +1346,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D5" s="4">
         <v>1</v>
       </c>
@@ -1336,7 +1357,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D6" s="4">
         <v>2</v>
       </c>
@@ -1347,7 +1368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D7" s="4">
         <v>4</v>
       </c>
@@ -1358,7 +1379,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D8" s="4">
         <v>6</v>
       </c>
@@ -1369,7 +1390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D9" s="4">
         <v>8</v>
       </c>
@@ -1380,7 +1401,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D10" s="4">
         <v>10</v>
       </c>
@@ -1391,7 +1412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D11" s="4">
         <v>13</v>
       </c>
@@ -1402,7 +1423,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D12" s="4">
         <v>15</v>
       </c>
@@ -1412,11 +1433,8 @@
       <c r="F12" s="5">
         <v>5</v>
       </c>
-      <c r="H12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D13" s="4">
         <v>19</v>
       </c>
@@ -1427,7 +1445,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D14" s="4">
         <v>23</v>
       </c>
@@ -1438,7 +1456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D15" s="4">
         <v>27</v>
       </c>
@@ -1449,7 +1467,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D16" s="4">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Practiced Cambridge 7 Test1 Listening.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D173D51-A086-45E7-9DB8-A0B96B956FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF54F242-9432-4FCB-BB47-D7EB0D352EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>IELTS17_Test4</t>
+  </si>
+  <si>
+    <t>IELTS7_Test1</t>
   </si>
 </sst>
 </file>
@@ -711,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1232,14 +1235,14 @@
         <v>6</v>
       </c>
       <c r="I20" s="12">
-        <v>1.1000000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="J20" s="9">
         <v>4</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="1"/>
-        <v>4.5250000000000004</v>
+        <v>5.625</v>
       </c>
     </row>
     <row r="21" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1264,14 +1267,14 @@
         <v>6.5</v>
       </c>
       <c r="I21" s="12">
-        <v>1.1000000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="J21" s="9">
         <v>4</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="1"/>
-        <v>4.7750000000000004</v>
+        <v>5.875</v>
       </c>
     </row>
     <row r="22" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1296,14 +1299,14 @@
         <v>5.5</v>
       </c>
       <c r="I22" s="12">
-        <v>1.1000000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="J22" s="9">
         <v>4</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="1"/>
-        <v>4.5250000000000004</v>
+        <v>5.875</v>
       </c>
     </row>
     <row r="23" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1328,14 +1331,14 @@
         <v>6</v>
       </c>
       <c r="I23" s="12">
-        <v>1.1000000000000001</v>
+        <v>6</v>
       </c>
       <c r="J23" s="9">
         <v>4</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="1"/>
-        <v>4.5250000000000004</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="24" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1360,22 +1363,33 @@
         <v>7.5</v>
       </c>
       <c r="I24" s="12">
-        <v>1.1000000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="J24" s="9">
         <v>4</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" ref="K24" si="2">(F24+H24+I24+J24)/4</f>
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="E25" s="6"/>
-      <c r="F25" s="10"/>
-      <c r="H25" s="11"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C25" s="13">
+        <v>45488</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="6">
+        <v>36</v>
+      </c>
+      <c r="F25" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
+      <c r="H25" s="9"/>
       <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Practiced Cambridge 7 Test 1 Reading.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF54F242-9432-4FCB-BB47-D7EB0D352EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EAFAFE-8BDA-4A12-9170-460CF71E6EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>IELTS7_Test1</t>
+  </si>
+  <si>
+    <t>IELTS9_Test1</t>
   </si>
 </sst>
 </file>
@@ -715,7 +718,7 @@
   <dimension ref="C1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1392,9 +1395,20 @@
       <c r="J25" s="9"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="E26" s="6"/>
-      <c r="F26" s="10"/>
+    <row r="26" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C26" s="13">
+        <v>45489</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="6">
+        <v>34</v>
+      </c>
+      <c r="F26" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7.5</v>
+      </c>
       <c r="H26" s="11"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>

</xml_diff>

<commit_message>
Practiced Cambridge 7 Test 1 & 2 Writing.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EAFAFE-8BDA-4A12-9170-460CF71E6EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99125D58-4DFF-4371-A38A-B7C53B17BE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>IELTS9_Test1</t>
+  </si>
+  <si>
+    <t>IELTS7_Test2</t>
   </si>
 </sst>
 </file>
@@ -718,7 +721,7 @@
   <dimension ref="C1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1391,7 +1394,9 @@
         <v>8</v>
       </c>
       <c r="H25" s="9"/>
-      <c r="I25" s="12"/>
+      <c r="I25" s="12">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="J25" s="9"/>
       <c r="K25" s="7"/>
     </row>
@@ -1414,11 +1419,24 @@
       <c r="J26" s="12"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="E27" s="6"/>
-      <c r="F27" s="10"/>
+    <row r="27" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C27" s="13">
+        <v>45492</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="6">
+        <v>30</v>
+      </c>
+      <c r="F27" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
       <c r="H27" s="11"/>
-      <c r="I27" s="12"/>
+      <c r="I27" s="12">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="J27" s="12"/>
       <c r="K27" s="7"/>
     </row>

</xml_diff>

<commit_message>
Cambridge 7 test 2 Practiced!
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99125D58-4DFF-4371-A38A-B7C53B17BE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A79F73-2D9D-45FB-ADCD-1A38F6F20DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>IELTS7_Test2</t>
+  </si>
+  <si>
+    <t>IELTS7_Test3</t>
+  </si>
+  <si>
+    <t>IELTS7_Test4</t>
   </si>
 </sst>
 </file>
@@ -721,7 +727,7 @@
   <dimension ref="C1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1393,7 +1399,13 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>8</v>
       </c>
-      <c r="H25" s="9"/>
+      <c r="G25">
+        <v>32</v>
+      </c>
+      <c r="H25" s="9">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
       <c r="I25" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -1414,7 +1426,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="7"/>
@@ -1433,22 +1445,40 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H27" s="11"/>
+      <c r="G27">
+        <v>24</v>
+      </c>
+      <c r="H27" s="9">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6</v>
+      </c>
       <c r="I27" s="12">
         <v>1.1000000000000001</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C28" s="13">
+        <v>45493</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
       <c r="E28" s="6"/>
-      <c r="F28" s="10"/>
+      <c r="F28" s="8"/>
       <c r="H28" s="11"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C29" s="13">
+        <v>45494</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
       <c r="E29" s="6"/>
       <c r="F29" s="10"/>
       <c r="H29" s="11"/>

</xml_diff>

<commit_message>
Cambridge 7 test 3 & 4 Practiced!
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A79F73-2D9D-45FB-ADCD-1A38F6F20DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2739522-E524-4B63-9002-DDBD3C4602FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,9 +261,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,7 +341,7 @@
         <color theme="3"/>
         <name val="Calibri"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -727,7 +729,7 @@
   <dimension ref="C1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,7 +741,7 @@
     <col min="5" max="5" width="6.7265625" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="6.54296875" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="7" customWidth="1"/>
     <col min="9" max="9" width="9.26953125" customWidth="1"/>
     <col min="10" max="10" width="10.08984375" customWidth="1"/>
     <col min="11" max="11" width="12.26953125" customWidth="1"/>
@@ -763,7 +765,7 @@
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -777,7 +779,7 @@
       </c>
     </row>
     <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>45419</v>
       </c>
       <c r="D4" t="s">
@@ -793,7 +795,7 @@
       <c r="G4">
         <v>13</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>4.5</v>
       </c>
@@ -807,7 +809,7 @@
       </c>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>45421</v>
       </c>
       <c r="D5" t="s">
@@ -820,7 +822,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9">
         <v>4</v>
@@ -831,7 +833,7 @@
       </c>
     </row>
     <row r="6" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>45428</v>
       </c>
       <c r="D6" t="s">
@@ -847,7 +849,7 @@
       <c r="G6">
         <v>20</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
@@ -863,7 +865,7 @@
       </c>
     </row>
     <row r="7" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>45429</v>
       </c>
       <c r="D7" t="s">
@@ -879,7 +881,7 @@
       <c r="G7">
         <v>20</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
@@ -895,7 +897,7 @@
       </c>
     </row>
     <row r="8" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>45431</v>
       </c>
       <c r="D8" t="s">
@@ -903,7 +905,7 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="8"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="9">
         <v>4.5</v>
       </c>
@@ -916,7 +918,7 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>45435</v>
       </c>
       <c r="D9" t="s">
@@ -927,7 +929,7 @@
       <c r="G9">
         <v>24</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
@@ -941,7 +943,7 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>45436</v>
       </c>
       <c r="D10" t="s">
@@ -957,7 +959,7 @@
       <c r="G10">
         <v>20</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
@@ -972,7 +974,7 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>45437</v>
       </c>
       <c r="D11" t="s">
@@ -980,7 +982,7 @@
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="9">
         <v>6</v>
       </c>
@@ -993,7 +995,7 @@
       </c>
     </row>
     <row r="12" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <v>45438</v>
       </c>
       <c r="D12" t="s">
@@ -1001,7 +1003,7 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="8"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="9">
         <v>4</v>
       </c>
@@ -1014,7 +1016,7 @@
       </c>
     </row>
     <row r="13" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <v>45443</v>
       </c>
       <c r="D13" t="s">
@@ -1025,7 +1027,7 @@
       <c r="G13">
         <v>25</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
@@ -1034,7 +1036,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>45447</v>
       </c>
       <c r="D14" t="s">
@@ -1050,7 +1052,7 @@
       <c r="G14">
         <v>28</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
@@ -1066,7 +1068,7 @@
       </c>
     </row>
     <row r="15" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="13">
+      <c r="C15" s="12">
         <v>45449</v>
       </c>
       <c r="D15" t="s">
@@ -1082,7 +1084,7 @@
       <c r="G15">
         <v>29</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
@@ -1098,7 +1100,7 @@
       </c>
     </row>
     <row r="16" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="13">
+      <c r="C16" s="12">
         <v>45452</v>
       </c>
       <c r="D16" t="s">
@@ -1114,7 +1116,7 @@
       <c r="G16">
         <v>26</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
@@ -1130,7 +1132,7 @@
       </c>
     </row>
     <row r="17" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="13">
+      <c r="C17" s="12">
         <v>45454</v>
       </c>
       <c r="D17" t="s">
@@ -1146,11 +1148,11 @@
       <c r="G17">
         <v>32</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <v>6.5</v>
       </c>
       <c r="J17" s="9">
@@ -1162,7 +1164,7 @@
       </c>
     </row>
     <row r="18" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <v>45456</v>
       </c>
       <c r="D18" t="s">
@@ -1178,11 +1180,11 @@
       <c r="G18">
         <v>24</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <v>6</v>
       </c>
       <c r="J18" s="9">
@@ -1194,7 +1196,7 @@
       </c>
     </row>
     <row r="19" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="13">
+      <c r="C19" s="12">
         <v>45457</v>
       </c>
       <c r="D19" t="s">
@@ -1210,11 +1212,11 @@
       <c r="G19">
         <v>25</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="11">
         <v>4</v>
       </c>
       <c r="J19" s="9">
@@ -1226,7 +1228,7 @@
       </c>
     </row>
     <row r="20" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <v>45466</v>
       </c>
       <c r="D20" t="s">
@@ -1242,11 +1244,11 @@
       <c r="G20">
         <v>26</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="11">
         <v>5.5</v>
       </c>
       <c r="J20" s="9">
@@ -1258,7 +1260,7 @@
       </c>
     </row>
     <row r="21" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="13">
+      <c r="C21" s="12">
         <v>45469</v>
       </c>
       <c r="D21" t="s">
@@ -1274,11 +1276,11 @@
       <c r="G21">
         <v>29</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="11">
         <v>5.5</v>
       </c>
       <c r="J21" s="9">
@@ -1290,7 +1292,7 @@
       </c>
     </row>
     <row r="22" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="13">
+      <c r="C22" s="12">
         <v>45471</v>
       </c>
       <c r="D22" t="s">
@@ -1306,11 +1308,11 @@
       <c r="G22">
         <v>22</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="11">
         <v>6.5</v>
       </c>
       <c r="J22" s="9">
@@ -1322,7 +1324,7 @@
       </c>
     </row>
     <row r="23" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="13">
+      <c r="C23" s="12">
         <v>45472</v>
       </c>
       <c r="D23" t="s">
@@ -1338,11 +1340,11 @@
       <c r="G23">
         <v>25</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="11">
         <v>6</v>
       </c>
       <c r="J23" s="9">
@@ -1354,7 +1356,7 @@
       </c>
     </row>
     <row r="24" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C24" s="13">
+      <c r="C24" s="12">
         <v>45473</v>
       </c>
       <c r="D24" t="s">
@@ -1370,11 +1372,11 @@
       <c r="G24">
         <v>34</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="11">
         <v>6.5</v>
       </c>
       <c r="J24" s="9">
@@ -1386,7 +1388,7 @@
       </c>
     </row>
     <row r="25" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="13">
+      <c r="C25" s="12">
         <v>45488</v>
       </c>
       <c r="D25" t="s">
@@ -1402,18 +1404,18 @@
       <c r="G25">
         <v>32</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="11">
         <v>1.1000000000000001</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="13">
+      <c r="C26" s="12">
         <v>45489</v>
       </c>
       <c r="D26" t="s">
@@ -1426,13 +1428,13 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C27" s="13">
+      <c r="C27" s="12">
         <v>45492</v>
       </c>
       <c r="D27" t="s">
@@ -1448,58 +1450,84 @@
       <c r="G27">
         <v>24</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I27" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J27" s="12"/>
+      <c r="J27" s="11"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C28" s="13">
+      <c r="C28" s="12">
         <v>45493</v>
       </c>
       <c r="D28" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="8"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
+      <c r="E28" s="6">
+        <v>32</v>
+      </c>
+      <c r="F28" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>32</v>
+      </c>
+      <c r="H28" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="I28" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J28" s="11"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C29" s="13">
+    <row r="29" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="12">
         <v>45494</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="10"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
+      <c r="E29" s="6">
+        <v>31</v>
+      </c>
+      <c r="F29" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>32</v>
+      </c>
+      <c r="H29" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="I29" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J29" s="11"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.35">
       <c r="E30" s="6"/>
       <c r="F30" s="10"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.35">
       <c r="E31" s="6"/>
       <c r="F31" s="10"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
       <c r="K31" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambridge 9 Test 2 Writing Practiced!
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2739522-E524-4B63-9002-DDBD3C4602FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937CBA8B-59CF-4FA5-8DB3-9AF3B00A8584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>IELTS7_Test4</t>
+  </si>
+  <si>
+    <t>IELTS9_Test2</t>
+  </si>
+  <si>
+    <t>No.</t>
   </si>
 </sst>
 </file>
@@ -241,7 +247,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,7 +268,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -272,6 +277,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -279,7 +296,14 @@
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="center"/>
@@ -371,23 +395,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:K31" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="C3:K31" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L41" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="C3:L41" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
+  <tableColumns count="10">
+    <tableColumn id="10" xr3:uid="{5AC48ABC-B60E-45DE-9969-4F077A234137}" name="No." dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{DC71C96E-388E-4427-9265-6CF875C8C5D7}" name="Course"/>
-    <tableColumn id="9" xr3:uid="{D3F721AC-61B7-43CC-AF2E-6E0AC12EB3B2}" name="Lis_Mark" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A705CE31-7A52-4C7A-85F3-5408CE0B0560}" name="Listening" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{D3F721AC-61B7-43CC-AF2E-6E0AC12EB3B2}" name="Lis_Mark" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{A705CE31-7A52-4C7A-85F3-5408CE0B0560}" name="Listening" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Lis_Mark]],Table3[[From]:[To]], 3, TRUE),"No Grade")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{65004197-C26E-4874-9A2E-3A56EC978737}" name="Read_Mark"/>
-    <tableColumn id="4" xr3:uid="{EF57AC4F-0BC5-47DA-A549-5E18B8D107B5}" name="Reading" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{EF57AC4F-0BC5-47DA-A549-5E18B8D107B5}" name="Reading" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15AFFB2A-07B5-47FC-9437-545D8A8916B1}" name="Writing" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{C0566DD1-3113-4CF0-96DC-1B3F892D0FAF}" name="Speaking" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{5E672D08-F03A-4519-AD28-B657B411A22F}" name="Overall" dataDxfId="5">
-      <calculatedColumnFormula>(F4+H4+I4+J4)/4</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{15AFFB2A-07B5-47FC-9437-545D8A8916B1}" name="Writing" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{C0566DD1-3113-4CF0-96DC-1B3F892D0FAF}" name="Speaking" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{5E672D08-F03A-4519-AD28-B657B411A22F}" name="Overall" dataDxfId="7">
+      <calculatedColumnFormula>(G4+I4+J4+K4)/4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -395,15 +420,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}" name="Table3" displayName="Table3" ref="D4:F20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}" name="Table3" displayName="Table3" ref="D4:F20" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="D4:F20" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:F20">
     <sortCondition ref="F4:F20"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2FE19739-2635-4933-9D55-4983D35E031D}" name="From" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A722DE31-0502-40CE-AE01-B2178E5F2D6E}" name="To" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{8081C4D8-49F2-41DD-A868-2F4234154D0E}" name="Band_Score" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2FE19739-2635-4933-9D55-4983D35E031D}" name="From" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{A722DE31-0502-40CE-AE01-B2178E5F2D6E}" name="To" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{8081C4D8-49F2-41DD-A868-2F4234154D0E}" name="Band_Score" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,809 +751,1000 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:M31"/>
+  <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.81640625" customWidth="1"/>
-    <col min="2" max="2" width="2.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="6.7265625" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="6.54296875" customWidth="1"/>
     <col min="8" max="8" width="10.1796875" style="7" customWidth="1"/>
     <col min="9" max="9" width="9.26953125" customWidth="1"/>
     <col min="10" max="10" width="10.08984375" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" customWidth="1"/>
+    <col min="11" max="11" width="10.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" ht="6.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="3:13" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C3" s="2" t="s">
+    <row r="1" spans="2:14" ht="6.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="2"/>
+      <c r="C3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="12">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18">
         <v>45419</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <v>26</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G4" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>13</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>4.5</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9">
-        <v>4</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" ref="K4:K17" si="0">(F4+H4+I4+J4)/4</f>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9">
+        <v>4</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" ref="L4:L17" si="0">(G4+I4+J4+K4)/4</f>
         <v>3.625</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="12">
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="16">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18">
         <v>45421</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>22</v>
       </c>
-      <c r="F5" s="8">
+      <c r="G5" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9">
-        <v>4</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="H5"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7">
         <f t="shared" si="0"/>
         <v>2.375</v>
       </c>
     </row>
-    <row r="6" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="12">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="16">
+        <v>3</v>
+      </c>
+      <c r="D6" s="18">
         <v>45428</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <v>32</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G6" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>20</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I6" s="9">
+      <c r="J6" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J6" s="9">
-        <v>4</v>
-      </c>
-      <c r="K6" s="7">
+      <c r="K6" s="9">
+        <v>4</v>
+      </c>
+      <c r="L6" s="7">
         <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="12">
+    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="16">
+        <v>4</v>
+      </c>
+      <c r="D7" s="18">
         <v>45429</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <v>32</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>20</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I7" s="9">
-        <v>4</v>
-      </c>
       <c r="J7" s="9">
         <v>4</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="9">
+        <v>4</v>
+      </c>
+      <c r="L7" s="7">
         <f t="shared" si="0"/>
         <v>5.125</v>
       </c>
     </row>
-    <row r="8" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="12">
+    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="16">
+        <v>5</v>
+      </c>
+      <c r="D8" s="18">
         <v>45431</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9">
+      <c r="F8" s="6"/>
+      <c r="G8" s="8"/>
+      <c r="H8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="9">
         <v>4.5</v>
       </c>
-      <c r="J8" s="9">
-        <v>4</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="K8" s="9">
+        <v>4</v>
+      </c>
+      <c r="L8" s="7">
         <f t="shared" si="0"/>
         <v>2.125</v>
       </c>
     </row>
-    <row r="9" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="12">
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="16">
+        <v>6</v>
+      </c>
+      <c r="D9" s="18">
         <v>45435</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="8"/>
-      <c r="G9">
+      <c r="F9" s="6"/>
+      <c r="G9" s="8"/>
+      <c r="H9">
         <v>24</v>
       </c>
-      <c r="H9" s="8">
+      <c r="I9" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9">
-        <v>4</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="7">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="12">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="16">
+        <v>7</v>
+      </c>
+      <c r="D10" s="18">
         <v>45436</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F10" s="6">
         <v>31</v>
       </c>
-      <c r="F10" s="8">
+      <c r="G10" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>20</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9">
-        <v>4</v>
-      </c>
-      <c r="K10" s="7">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9">
+        <v>4</v>
+      </c>
+      <c r="L10" s="7">
         <f t="shared" si="0"/>
         <v>4.125</v>
       </c>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="12">
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="16">
+        <v>8</v>
+      </c>
+      <c r="D11" s="18">
         <v>45437</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9">
+      <c r="F11" s="6"/>
+      <c r="G11" s="8"/>
+      <c r="H11"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="9">
         <v>6</v>
       </c>
-      <c r="J11" s="9">
-        <v>4</v>
-      </c>
-      <c r="K11" s="7">
+      <c r="K11" s="9">
+        <v>4</v>
+      </c>
+      <c r="L11" s="7">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="12">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="16">
+        <v>9</v>
+      </c>
+      <c r="D12" s="18">
         <v>45438</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9">
-        <v>4</v>
-      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="8"/>
+      <c r="H12"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="9">
         <v>4</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="9">
+        <v>4</v>
+      </c>
+      <c r="L12" s="7">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="12">
+    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="16">
+        <v>10</v>
+      </c>
+      <c r="D13" s="18">
         <v>45443</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
-      <c r="G13">
+      <c r="F13" s="6"/>
+      <c r="G13" s="8"/>
+      <c r="H13">
         <v>25</v>
       </c>
-      <c r="H13" s="8">
+      <c r="I13" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="12">
+      <c r="K13" s="9"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C14" s="16">
+        <v>11</v>
+      </c>
+      <c r="D14" s="18">
         <v>45447</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="6">
+      <c r="F14" s="6">
         <v>30</v>
       </c>
-      <c r="F14" s="8">
+      <c r="G14" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>28</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I14" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="I14" s="9">
+      <c r="J14" s="9">
         <v>6.5</v>
       </c>
-      <c r="J14" s="9">
-        <v>4</v>
-      </c>
-      <c r="K14" s="7">
+      <c r="K14" s="9">
+        <v>4</v>
+      </c>
+      <c r="L14" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="12">
+    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C15" s="16">
+        <v>12</v>
+      </c>
+      <c r="D15" s="18">
         <v>45449</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F15" s="6">
         <v>34</v>
       </c>
-      <c r="F15" s="8">
+      <c r="G15" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>29</v>
       </c>
-      <c r="H15" s="8">
+      <c r="I15" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="I15" s="9">
+      <c r="J15" s="9">
         <v>5.5</v>
       </c>
-      <c r="J15" s="9">
-        <v>4</v>
-      </c>
-      <c r="K15" s="7">
+      <c r="K15" s="9">
+        <v>4</v>
+      </c>
+      <c r="L15" s="7">
         <f t="shared" si="0"/>
         <v>5.875</v>
       </c>
     </row>
-    <row r="16" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="12">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C16" s="16">
+        <v>13</v>
+      </c>
+      <c r="D16" s="18">
         <v>45452</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="6">
+      <c r="F16" s="6">
         <v>30</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G16" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>26</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I16" s="9">
+      <c r="J16" s="9">
         <v>5</v>
       </c>
-      <c r="J16" s="9">
-        <v>4</v>
-      </c>
-      <c r="K16" s="7">
+      <c r="K16" s="9">
+        <v>4</v>
+      </c>
+      <c r="L16" s="7">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="12">
+    <row r="17" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="16">
+        <v>14</v>
+      </c>
+      <c r="D17" s="18">
         <v>45454</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="6">
         <v>33</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>32</v>
       </c>
-      <c r="H17" s="8">
+      <c r="I17" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="I17" s="11">
+      <c r="J17" s="11">
         <v>6.5</v>
       </c>
-      <c r="J17" s="9">
-        <v>4</v>
-      </c>
-      <c r="K17" s="7">
+      <c r="K17" s="9">
+        <v>4</v>
+      </c>
+      <c r="L17" s="7">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="12">
+    <row r="18" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="16">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18">
         <v>45456</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="6">
+      <c r="F18" s="6">
         <v>33</v>
       </c>
-      <c r="F18" s="8">
+      <c r="G18" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>24</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I18" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I18" s="11">
+      <c r="J18" s="11">
         <v>6</v>
       </c>
-      <c r="J18" s="9">
-        <v>4</v>
-      </c>
-      <c r="K18" s="7">
-        <f t="shared" ref="K18:K23" si="1">(F18+H18+I18+J18)/4</f>
+      <c r="K18" s="9">
+        <v>4</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" ref="L18:L23" si="1">(G18+I18+J18+K18)/4</f>
         <v>5.875</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="12">
+    <row r="19" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C19" s="16">
+        <v>16</v>
+      </c>
+      <c r="D19" s="18">
         <v>45457</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="6">
+      <c r="F19" s="6">
         <v>29</v>
       </c>
-      <c r="F19" s="8">
+      <c r="G19" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>25</v>
       </c>
-      <c r="H19" s="8">
+      <c r="I19" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I19" s="11">
-        <v>4</v>
-      </c>
-      <c r="J19" s="9">
-        <v>4</v>
-      </c>
-      <c r="K19" s="7">
+      <c r="J19" s="11">
+        <v>4</v>
+      </c>
+      <c r="K19" s="9">
+        <v>4</v>
+      </c>
+      <c r="L19" s="7">
         <f t="shared" si="1"/>
         <v>5.125</v>
       </c>
     </row>
-    <row r="20" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="12">
+    <row r="20" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="16">
+        <v>17</v>
+      </c>
+      <c r="D20" s="18">
         <v>45466</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="6">
+      <c r="F20" s="6">
         <v>32</v>
       </c>
-      <c r="F20" s="8">
+      <c r="G20" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>26</v>
       </c>
-      <c r="H20" s="8">
+      <c r="I20" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I20" s="11">
+      <c r="J20" s="11">
         <v>5.5</v>
       </c>
-      <c r="J20" s="9">
-        <v>4</v>
-      </c>
-      <c r="K20" s="7">
+      <c r="K20" s="9">
+        <v>4</v>
+      </c>
+      <c r="L20" s="7">
         <f t="shared" si="1"/>
         <v>5.625</v>
       </c>
     </row>
-    <row r="21" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="12">
+    <row r="21" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C21" s="16">
+        <v>18</v>
+      </c>
+      <c r="D21" s="18">
         <v>45469</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="6">
+      <c r="F21" s="6">
         <v>34</v>
       </c>
-      <c r="F21" s="8">
+      <c r="G21" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>29</v>
       </c>
-      <c r="H21" s="8">
+      <c r="I21" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="I21" s="11">
+      <c r="J21" s="11">
         <v>5.5</v>
       </c>
-      <c r="J21" s="9">
-        <v>4</v>
-      </c>
-      <c r="K21" s="7">
+      <c r="K21" s="9">
+        <v>4</v>
+      </c>
+      <c r="L21" s="7">
         <f t="shared" si="1"/>
         <v>5.875</v>
       </c>
     </row>
-    <row r="22" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="12">
+    <row r="22" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C22" s="16">
+        <v>19</v>
+      </c>
+      <c r="D22" s="18">
         <v>45471</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="6">
+      <c r="F22" s="6">
         <v>34</v>
       </c>
-      <c r="F22" s="8">
+      <c r="G22" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>22</v>
       </c>
-      <c r="H22" s="8">
+      <c r="I22" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="I22" s="11">
+      <c r="J22" s="11">
         <v>6.5</v>
       </c>
-      <c r="J22" s="9">
-        <v>4</v>
-      </c>
-      <c r="K22" s="7">
+      <c r="K22" s="9">
+        <v>4</v>
+      </c>
+      <c r="L22" s="7">
         <f t="shared" si="1"/>
         <v>5.875</v>
       </c>
     </row>
-    <row r="23" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="12">
+    <row r="23" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C23" s="16">
+        <v>20</v>
+      </c>
+      <c r="D23" s="18">
         <v>45472</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="6">
+      <c r="F23" s="6">
         <v>31</v>
       </c>
-      <c r="F23" s="8">
+      <c r="G23" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>25</v>
       </c>
-      <c r="H23" s="8">
+      <c r="I23" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I23" s="11">
+      <c r="J23" s="11">
         <v>6</v>
       </c>
-      <c r="J23" s="9">
-        <v>4</v>
-      </c>
-      <c r="K23" s="7">
+      <c r="K23" s="9">
+        <v>4</v>
+      </c>
+      <c r="L23" s="7">
         <f t="shared" si="1"/>
         <v>5.75</v>
       </c>
     </row>
-    <row r="24" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C24" s="12">
+    <row r="24" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C24" s="16">
+        <v>21</v>
+      </c>
+      <c r="D24" s="18">
         <v>45473</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="6">
+      <c r="F24" s="6">
         <v>31</v>
       </c>
-      <c r="F24" s="8">
+      <c r="G24" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>34</v>
       </c>
-      <c r="H24" s="8">
+      <c r="I24" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="I24" s="11">
+      <c r="J24" s="11">
         <v>6.5</v>
       </c>
-      <c r="J24" s="9">
-        <v>4</v>
-      </c>
-      <c r="K24" s="7">
-        <f t="shared" ref="K24" si="2">(F24+H24+I24+J24)/4</f>
+      <c r="K24" s="9">
+        <v>4</v>
+      </c>
+      <c r="L24" s="7">
+        <f t="shared" ref="L24" si="2">(G24+I24+J24+K24)/4</f>
         <v>6.25</v>
       </c>
     </row>
-    <row r="25" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="12">
+    <row r="25" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C25" s="16">
+        <v>22</v>
+      </c>
+      <c r="D25" s="18">
         <v>45488</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="6">
+      <c r="F25" s="6">
         <v>36</v>
       </c>
-      <c r="F25" s="8">
+      <c r="G25" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>8</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>32</v>
       </c>
-      <c r="H25" s="8">
+      <c r="I25" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="I25" s="11">
+      <c r="J25" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="12">
+      <c r="K25" s="9"/>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C26" s="16">
+        <v>23</v>
+      </c>
+      <c r="D26" s="18">
         <v>45489</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="6">
+      <c r="F26" s="6">
         <v>34</v>
       </c>
-      <c r="F26" s="8">
+      <c r="G26" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="11"/>
+      <c r="H26"/>
+      <c r="I26" s="8"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C27" s="12">
+      <c r="K26" s="11"/>
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C27" s="16">
+        <v>24</v>
+      </c>
+      <c r="D27" s="18">
         <v>45492</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="6">
+      <c r="F27" s="6">
         <v>30</v>
       </c>
-      <c r="F27" s="8">
+      <c r="G27" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>24</v>
       </c>
-      <c r="H27" s="8">
+      <c r="I27" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="I27" s="11">
+      <c r="J27" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C28" s="12">
+      <c r="K27" s="11"/>
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C28" s="16">
+        <v>25</v>
+      </c>
+      <c r="D28" s="18">
         <v>45493</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="6">
+      <c r="F28" s="6">
         <v>32</v>
       </c>
-      <c r="F28" s="8">
+      <c r="G28" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>32</v>
       </c>
-      <c r="H28" s="8">
+      <c r="I28" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="I28" s="11">
+      <c r="J28" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="12">
+      <c r="K28" s="11"/>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="16">
+        <v>26</v>
+      </c>
+      <c r="D29" s="18">
         <v>45494</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="6">
+      <c r="F29" s="6">
         <v>31</v>
       </c>
-      <c r="F29" s="8">
+      <c r="G29" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>32</v>
       </c>
-      <c r="H29" s="8">
+      <c r="I29" s="8">
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="I29" s="11">
+      <c r="J29" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J29" s="11"/>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="E30" s="6"/>
-      <c r="F30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="E31" s="6"/>
-      <c r="F31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C30" s="16">
+        <v>27</v>
+      </c>
+      <c r="D30" s="18">
+        <v>45495</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="8"/>
+      <c r="H30"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="7"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="F31" s="6"/>
+      <c r="G31" s="10"/>
+      <c r="H31"/>
+      <c r="I31" s="10"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="7"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="7"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="F32" s="6"/>
+      <c r="G32" s="10"/>
+      <c r="H32"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="7"/>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F33" s="6"/>
+      <c r="G33" s="10"/>
+      <c r="H33"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="7"/>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F34" s="6"/>
+      <c r="G34" s="10"/>
+      <c r="H34"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="7"/>
+    </row>
+    <row r="35" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F35" s="6"/>
+      <c r="G35" s="10"/>
+      <c r="H35"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="7"/>
+    </row>
+    <row r="36" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F36" s="6"/>
+      <c r="G36" s="10"/>
+      <c r="H36"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="7"/>
+    </row>
+    <row r="37" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F37" s="6"/>
+      <c r="G37" s="10"/>
+      <c r="H37"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="7"/>
+    </row>
+    <row r="38" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F38" s="6"/>
+      <c r="G38" s="10"/>
+      <c r="H38"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="7"/>
+    </row>
+    <row r="39" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F39" s="6"/>
+      <c r="G39" s="10"/>
+      <c r="H39"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="7"/>
+    </row>
+    <row r="40" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F40" s="6"/>
+      <c r="G40" s="10"/>
+      <c r="H40"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="7"/>
+    </row>
+    <row r="41" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F41" s="6"/>
+      <c r="G41" s="10"/>
+      <c r="H41"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1555,17 +1771,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="14"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Writing Grades inserted to Score table!
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937CBA8B-59CF-4FA5-8DB3-9AF3B00A8584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E5B31C-6B18-4373-9AF2-BAB89C859BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,22 +271,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -297,13 +291,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="center"/>
@@ -379,6 +366,13 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center"/>
     </dxf>
   </dxfs>
@@ -398,20 +392,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L41" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="C3:L41" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
   <tableColumns count="10">
-    <tableColumn id="10" xr3:uid="{5AC48ABC-B60E-45DE-9969-4F077A234137}" name="No." dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{5AC48ABC-B60E-45DE-9969-4F077A234137}" name="No." dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{DC71C96E-388E-4427-9265-6CF875C8C5D7}" name="Course"/>
-    <tableColumn id="9" xr3:uid="{D3F721AC-61B7-43CC-AF2E-6E0AC12EB3B2}" name="Lis_Mark" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{A705CE31-7A52-4C7A-85F3-5408CE0B0560}" name="Listening" dataDxfId="11">
+    <tableColumn id="9" xr3:uid="{D3F721AC-61B7-43CC-AF2E-6E0AC12EB3B2}" name="Lis_Mark" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A705CE31-7A52-4C7A-85F3-5408CE0B0560}" name="Listening" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Lis_Mark]],Table3[[From]:[To]], 3, TRUE),"No Grade")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{65004197-C26E-4874-9A2E-3A56EC978737}" name="Read_Mark"/>
-    <tableColumn id="4" xr3:uid="{EF57AC4F-0BC5-47DA-A549-5E18B8D107B5}" name="Reading" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{EF57AC4F-0BC5-47DA-A549-5E18B8D107B5}" name="Reading" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15AFFB2A-07B5-47FC-9437-545D8A8916B1}" name="Writing" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{C0566DD1-3113-4CF0-96DC-1B3F892D0FAF}" name="Speaking" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{5E672D08-F03A-4519-AD28-B657B411A22F}" name="Overall" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{15AFFB2A-07B5-47FC-9437-545D8A8916B1}" name="Writing" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C0566DD1-3113-4CF0-96DC-1B3F892D0FAF}" name="Speaking" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{5E672D08-F03A-4519-AD28-B657B411A22F}" name="Overall" dataDxfId="5">
       <calculatedColumnFormula>(G4+I4+J4+K4)/4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -420,15 +414,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}" name="Table3" displayName="Table3" ref="D4:F20" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}" name="Table3" displayName="Table3" ref="D4:F20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="D4:F20" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:F20">
     <sortCondition ref="F4:F20"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2FE19739-2635-4933-9D55-4983D35E031D}" name="From" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{A722DE31-0502-40CE-AE01-B2178E5F2D6E}" name="To" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{8081C4D8-49F2-41DD-A868-2F4234154D0E}" name="Band_Score" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2FE19739-2635-4933-9D55-4983D35E031D}" name="From" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A722DE31-0502-40CE-AE01-B2178E5F2D6E}" name="To" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{8081C4D8-49F2-41DD-A868-2F4234154D0E}" name="Band_Score" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -753,16 +747,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.81640625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="13" customWidth="1"/>
     <col min="5" max="5" width="15.26953125" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="6.54296875" customWidth="1"/>
@@ -777,7 +771,7 @@
     <row r="2" spans="2:14" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -809,10 +803,10 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="16">
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="14">
         <v>45419</v>
       </c>
       <c r="E4" t="s">
@@ -842,10 +836,10 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <v>2</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="14">
         <v>45421</v>
       </c>
       <c r="E5" t="s">
@@ -870,10 +864,10 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>3</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="14">
         <v>45428</v>
       </c>
       <c r="E6" t="s">
@@ -905,10 +899,10 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="16">
-        <v>4</v>
-      </c>
-      <c r="D7" s="18">
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14">
         <v>45429</v>
       </c>
       <c r="E7" t="s">
@@ -940,10 +934,10 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>5</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>45431</v>
       </c>
       <c r="E8" t="s">
@@ -965,10 +959,10 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <v>6</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="14">
         <v>45435</v>
       </c>
       <c r="E9" t="s">
@@ -993,10 +987,10 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>7</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="14">
         <v>45436</v>
       </c>
       <c r="E10" t="s">
@@ -1027,10 +1021,10 @@
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <v>8</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="14">
         <v>45437</v>
       </c>
       <c r="E11" t="s">
@@ -1052,10 +1046,10 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <v>9</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="14">
         <v>45438</v>
       </c>
       <c r="E12" t="s">
@@ -1077,10 +1071,10 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="16">
+      <c r="C13" s="13">
         <v>10</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="14">
         <v>45443</v>
       </c>
       <c r="E13" t="s">
@@ -1100,10 +1094,10 @@
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="16">
+      <c r="C14" s="13">
         <v>11</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="14">
         <v>45447</v>
       </c>
       <c r="E14" t="s">
@@ -1135,10 +1129,10 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <v>12</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="14">
         <v>45449</v>
       </c>
       <c r="E15" t="s">
@@ -1170,10 +1164,10 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="16">
+      <c r="C16" s="13">
         <v>13</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="14">
         <v>45452</v>
       </c>
       <c r="E16" t="s">
@@ -1205,10 +1199,10 @@
       </c>
     </row>
     <row r="17" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="16">
+      <c r="C17" s="13">
         <v>14</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="14">
         <v>45454</v>
       </c>
       <c r="E17" t="s">
@@ -1240,10 +1234,10 @@
       </c>
     </row>
     <row r="18" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="16">
+      <c r="C18" s="13">
         <v>15</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="14">
         <v>45456</v>
       </c>
       <c r="E18" t="s">
@@ -1275,10 +1269,10 @@
       </c>
     </row>
     <row r="19" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="16">
+      <c r="C19" s="13">
         <v>16</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="14">
         <v>45457</v>
       </c>
       <c r="E19" t="s">
@@ -1310,10 +1304,10 @@
       </c>
     </row>
     <row r="20" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="16">
+      <c r="C20" s="13">
         <v>17</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="14">
         <v>45466</v>
       </c>
       <c r="E20" t="s">
@@ -1345,10 +1339,10 @@
       </c>
     </row>
     <row r="21" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="16">
+      <c r="C21" s="13">
         <v>18</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="14">
         <v>45469</v>
       </c>
       <c r="E21" t="s">
@@ -1380,10 +1374,10 @@
       </c>
     </row>
     <row r="22" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="16">
+      <c r="C22" s="13">
         <v>19</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="14">
         <v>45471</v>
       </c>
       <c r="E22" t="s">
@@ -1415,10 +1409,10 @@
       </c>
     </row>
     <row r="23" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="16">
+      <c r="C23" s="13">
         <v>20</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="14">
         <v>45472</v>
       </c>
       <c r="E23" t="s">
@@ -1450,10 +1444,10 @@
       </c>
     </row>
     <row r="24" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C24" s="16">
+      <c r="C24" s="13">
         <v>21</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="14">
         <v>45473</v>
       </c>
       <c r="E24" t="s">
@@ -1480,15 +1474,15 @@
         <v>4</v>
       </c>
       <c r="L24" s="7">
-        <f t="shared" ref="L24" si="2">(G24+I24+J24+K24)/4</f>
+        <f t="shared" ref="L24:L30" si="2">(G24+I24+J24+K24)/4</f>
         <v>6.25</v>
       </c>
     </row>
     <row r="25" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="16">
+      <c r="C25" s="13">
         <v>22</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="14">
         <v>45488</v>
       </c>
       <c r="E25" t="s">
@@ -1509,16 +1503,21 @@
         <v>7</v>
       </c>
       <c r="J25" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="K25" s="9">
+        <v>4</v>
+      </c>
+      <c r="L25" s="7">
+        <f t="shared" si="2"/>
+        <v>6.125</v>
+      </c>
     </row>
     <row r="26" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="16">
+      <c r="C26" s="13">
         <v>23</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="14">
         <v>45489</v>
       </c>
       <c r="E26" t="s">
@@ -1534,14 +1533,19 @@
       <c r="H26"/>
       <c r="I26" s="8"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="7"/>
+      <c r="K26" s="9">
+        <v>4</v>
+      </c>
+      <c r="L26" s="7">
+        <f t="shared" si="2"/>
+        <v>2.875</v>
+      </c>
     </row>
     <row r="27" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C27" s="16">
+      <c r="C27" s="13">
         <v>24</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="14">
         <v>45492</v>
       </c>
       <c r="E27" t="s">
@@ -1562,16 +1566,21 @@
         <v>6</v>
       </c>
       <c r="J27" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="K27" s="9">
+        <v>4</v>
+      </c>
+      <c r="L27" s="7">
+        <f t="shared" si="2"/>
+        <v>5.625</v>
+      </c>
     </row>
     <row r="28" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C28" s="16">
+      <c r="C28" s="13">
         <v>25</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="14">
         <v>45493</v>
       </c>
       <c r="E28" t="s">
@@ -1592,16 +1601,21 @@
         <v>7</v>
       </c>
       <c r="J28" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="K28" s="9">
+        <v>4</v>
+      </c>
+      <c r="L28" s="7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="16">
+      <c r="C29" s="13">
         <v>26</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="14">
         <v>45494</v>
       </c>
       <c r="E29" t="s">
@@ -1622,16 +1636,21 @@
         <v>7</v>
       </c>
       <c r="J29" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="K29" s="9">
+        <v>4</v>
+      </c>
+      <c r="L29" s="7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="30" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C30" s="16">
+      <c r="C30" s="13">
         <v>27</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="14">
         <v>45495</v>
       </c>
       <c r="E30" t="s">
@@ -1642,10 +1661,15 @@
       <c r="H30"/>
       <c r="I30" s="8"/>
       <c r="J30" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K30" s="11"/>
-      <c r="L30" s="7"/>
+        <v>6.5</v>
+      </c>
+      <c r="K30" s="9">
+        <v>4</v>
+      </c>
+      <c r="L30" s="7">
+        <f t="shared" si="2"/>
+        <v>2.625</v>
+      </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F31" s="6"/>
@@ -1771,17 +1795,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Practiced Test 1 reading Test 2 Listening.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7C0EE-5660-41D3-ABCF-ABC968BF787F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC57514-CCC6-46FE-B35D-F394088B7D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t>IELTS9_Test3</t>
+  </si>
+  <si>
+    <t>IELTS9_Test4</t>
   </si>
 </sst>
 </file>
@@ -747,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -764,7 +770,7 @@
     <col min="9" max="9" width="9.26953125" customWidth="1"/>
     <col min="10" max="10" width="10.08984375" customWidth="1"/>
     <col min="11" max="11" width="10.54296875" customWidth="1"/>
-    <col min="12" max="12" width="12.90625" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="6.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1041,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="7">
-        <f t="shared" si="0"/>
+        <f>(G11+I11+J11+K11)/4</f>
         <v>2.75</v>
       </c>
     </row>
@@ -1066,7 +1072,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="7">
-        <f t="shared" si="0"/>
+        <f>(G12+I12+J12+K12)/4</f>
         <v>2.25</v>
       </c>
     </row>
@@ -1532,15 +1538,20 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H26"/>
-      <c r="I26" s="8"/>
+      <c r="H26">
+        <v>27</v>
+      </c>
+      <c r="I26" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
       <c r="J26" s="11"/>
       <c r="K26" s="9">
         <v>5</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="2"/>
-        <v>3.125</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="27" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1658,8 +1669,13 @@
       <c r="E30" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="8"/>
+      <c r="F30" s="6">
+        <v>35</v>
+      </c>
+      <c r="G30" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
       <c r="H30"/>
       <c r="I30" s="8"/>
       <c r="J30" s="11">
@@ -1670,10 +1686,19 @@
       </c>
       <c r="L30" s="7">
         <f t="shared" si="2"/>
-        <v>2.875</v>
+        <v>4.875</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="13">
+        <v>28</v>
+      </c>
+      <c r="D31" s="14">
+        <v>45504</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="10"/>
       <c r="H31"/>
@@ -1683,6 +1708,15 @@
       <c r="L31" s="7"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="13">
+        <v>29</v>
+      </c>
+      <c r="D32" s="14">
+        <v>45505</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="10"/>
       <c r="H32"/>

</xml_diff>

<commit_message>
Practiced Cambridge 9 Test 4.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C4F7A5-1C63-4520-9EA3-F5DCF5B614A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6EBC74-5A74-498E-B73A-E9E6031F99E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -754,7 +754,7 @@
   <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1676,8 +1676,13 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>8</v>
       </c>
-      <c r="H30"/>
-      <c r="I30" s="8"/>
+      <c r="H30">
+        <v>32</v>
+      </c>
+      <c r="I30" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
       <c r="J30" s="11">
         <v>6.5</v>
       </c>
@@ -1686,7 +1691,7 @@
       </c>
       <c r="L30" s="7">
         <f t="shared" si="2"/>
-        <v>4.875</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="31" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1719,21 +1724,33 @@
       <c r="K31" s="11"/>
       <c r="L31" s="7"/>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="13">
         <v>29</v>
       </c>
       <c r="D32" s="14">
-        <v>45505</v>
+        <v>45508</v>
       </c>
       <c r="E32" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="10"/>
-      <c r="H32"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="11"/>
+      <c r="F32" s="6">
+        <v>33</v>
+      </c>
+      <c r="G32" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7.5</v>
+      </c>
+      <c r="H32">
+        <v>29</v>
+      </c>
+      <c r="I32" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
+      <c r="J32" s="11">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="K32" s="11"/>
       <c r="L32" s="7"/>
     </row>

</xml_diff>

<commit_message>
Cambridge 13 test 3 Writing Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC3C595-64A3-482F-9C2E-298AB09127F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2083C-E42B-42B2-99E3-86F652610C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>IELTS9_Test4</t>
+  </si>
+  <si>
+    <t>IELTS13_Test1</t>
+  </si>
+  <si>
+    <t>IELTS13_Test2</t>
+  </si>
+  <si>
+    <t>IELTS13_Test3</t>
+  </si>
+  <si>
+    <t>IELTS13_Test4</t>
   </si>
 </sst>
 </file>
@@ -754,7 +766,7 @@
   <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1764,43 +1776,85 @@
         <v>5.0250000000000004</v>
       </c>
     </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C33" s="13">
+        <v>30</v>
+      </c>
+      <c r="D33" s="14">
+        <v>45512</v>
+      </c>
+      <c r="E33" t="s">
+        <v>40</v>
+      </c>
       <c r="F33" s="6"/>
-      <c r="G33" s="10"/>
+      <c r="G33" s="8"/>
       <c r="H33"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K33" s="9"/>
       <c r="L33" s="7"/>
     </row>
-    <row r="34" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C34" s="13">
+        <v>31</v>
+      </c>
+      <c r="D34" s="14">
+        <v>45513</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
       <c r="F34" s="6"/>
-      <c r="G34" s="10"/>
+      <c r="G34" s="8"/>
       <c r="H34"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K34" s="9"/>
       <c r="L34" s="7"/>
     </row>
-    <row r="35" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="13">
+        <v>32</v>
+      </c>
+      <c r="D35" s="14">
+        <v>45514</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
       <c r="F35" s="6"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="8"/>
       <c r="H35"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K35" s="9"/>
       <c r="L35" s="7"/>
     </row>
-    <row r="36" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C36" s="13">
+        <v>33</v>
+      </c>
+      <c r="D36" s="14">
+        <v>45515</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
       <c r="F36" s="6"/>
-      <c r="G36" s="10"/>
+      <c r="G36" s="8"/>
       <c r="H36"/>
-      <c r="I36" s="10"/>
+      <c r="I36" s="8"/>
       <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
+      <c r="K36" s="9"/>
       <c r="L36" s="7"/>
     </row>
-    <row r="37" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F37" s="6"/>
       <c r="G37" s="10"/>
       <c r="H37"/>
@@ -1809,7 +1863,7 @@
       <c r="K37" s="11"/>
       <c r="L37" s="7"/>
     </row>
-    <row r="38" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F38" s="6"/>
       <c r="G38" s="10"/>
       <c r="H38"/>
@@ -1818,7 +1872,7 @@
       <c r="K38" s="11"/>
       <c r="L38" s="7"/>
     </row>
-    <row r="39" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F39" s="6"/>
       <c r="G39" s="10"/>
       <c r="H39"/>
@@ -1827,7 +1881,7 @@
       <c r="K39" s="11"/>
       <c r="L39" s="7"/>
     </row>
-    <row r="40" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F40" s="6"/>
       <c r="G40" s="10"/>
       <c r="H40"/>
@@ -1836,7 +1890,7 @@
       <c r="K40" s="11"/>
       <c r="L40" s="7"/>
     </row>
-    <row r="41" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F41" s="6"/>
       <c r="G41" s="10"/>
       <c r="H41"/>

</xml_diff>

<commit_message>
Cambridge 13 test 3 Reading Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25715B43-811B-455B-9658-DA607CC683F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A30C96B-0D4A-4952-B9EF-11C2A9631DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -766,7 +766,7 @@
   <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1857,8 +1857,13 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H35"/>
-      <c r="I35" s="8"/>
+      <c r="H35">
+        <v>34</v>
+      </c>
+      <c r="I35" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7.5</v>
+      </c>
       <c r="J35" s="11">
         <v>1.1000000000000001</v>
       </c>

</xml_diff>

<commit_message>
Cambridge 13 test 4 Listening Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A30C96B-0D4A-4952-B9EF-11C2A9631DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C23141-15D5-47A1-A377-43C76905FF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -766,7 +766,7 @@
   <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1882,8 +1882,13 @@
       <c r="E36" t="s">
         <v>43</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="8"/>
+      <c r="F36" s="6">
+        <v>30</v>
+      </c>
+      <c r="G36" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
       <c r="H36"/>
       <c r="I36" s="8"/>
       <c r="J36" s="11"/>

</xml_diff>

<commit_message>
Cambridge 13 test 4 Reading Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C23141-15D5-47A1-A377-43C76905FF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40C2E19-B744-429E-8C49-A8F377B36397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -766,7 +766,7 @@
   <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1889,10 +1889,17 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H36"/>
-      <c r="I36" s="8"/>
+      <c r="H36">
+        <v>27</v>
+      </c>
+      <c r="I36" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
       <c r="J36" s="11"/>
-      <c r="K36" s="9"/>
+      <c r="K36" s="9">
+        <v>5</v>
+      </c>
       <c r="L36" s="7"/>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Cambridge 9 Writing Score added.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40C2E19-B744-429E-8C49-A8F377B36397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD835A6C-9DA3-47ED-8C4C-83BF42900ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -766,7 +766,7 @@
   <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1766,14 +1766,14 @@
         <v>6.5</v>
       </c>
       <c r="J32" s="11">
-        <v>1.1000000000000001</v>
+        <v>6</v>
       </c>
       <c r="K32" s="9">
         <v>5</v>
       </c>
       <c r="L32" s="7">
         <f t="shared" si="2"/>
-        <v>5.0250000000000004</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="33" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1896,7 +1896,9 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="J36" s="11"/>
+      <c r="J36" s="11">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="K36" s="9">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
McCarter & Ash Reading Test 1 Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD835A6C-9DA3-47ED-8C4C-83BF42900ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE5FF6D-162D-4502-A1AB-AF384D610C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>IELTS13_Test4</t>
+  </si>
+  <si>
+    <t>McCarter&amp;Ash Test 1</t>
   </si>
 </sst>
 </file>
@@ -265,7 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,6 +302,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,8 +413,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L41" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="C3:L41" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L53" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="C3:L53" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{5AC48ABC-B60E-45DE-9969-4F077A234137}" name="No." dataDxfId="12"/>
     <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date" dataDxfId="11"/>
@@ -763,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N41"/>
+  <dimension ref="B1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -775,7 +781,7 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="6.54296875" style="13" customWidth="1"/>
     <col min="4" max="4" width="12.90625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="6.54296875" customWidth="1"/>
     <col min="8" max="8" width="10.1796875" style="7" customWidth="1"/>
@@ -1494,7 +1500,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="7">
-        <f t="shared" ref="L24:L32" si="2">(G24+I24+J24+K24)/4</f>
+        <f t="shared" ref="L24:L36" si="2">(G24+I24+J24+K24)/4</f>
         <v>6.5</v>
       </c>
     </row>
@@ -1806,7 +1812,10 @@
       <c r="K33" s="9">
         <v>5</v>
       </c>
-      <c r="L33" s="7"/>
+      <c r="L33" s="7">
+        <f t="shared" si="2"/>
+        <v>5.2750000000000004</v>
+      </c>
     </row>
     <row r="34" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="13">
@@ -1838,7 +1847,10 @@
       <c r="K34" s="9">
         <v>5</v>
       </c>
-      <c r="L34" s="7"/>
+      <c r="L34" s="7">
+        <f t="shared" si="2"/>
+        <v>5.2750000000000004</v>
+      </c>
     </row>
     <row r="35" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="13">
@@ -1870,7 +1882,10 @@
       <c r="K35" s="9">
         <v>5</v>
       </c>
-      <c r="L35" s="7"/>
+      <c r="L35" s="7">
+        <f t="shared" si="2"/>
+        <v>5.15</v>
+      </c>
     </row>
     <row r="36" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" s="13">
@@ -1902,11 +1917,28 @@
       <c r="K36" s="9">
         <v>5</v>
       </c>
-      <c r="L36" s="7"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="F37" s="6"/>
-      <c r="G37" s="10"/>
+      <c r="L36" s="7">
+        <f t="shared" si="2"/>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C37" s="13">
+        <v>34</v>
+      </c>
+      <c r="D37" s="14">
+        <v>45517</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="6">
+        <v>24</v>
+      </c>
+      <c r="G37" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6</v>
+      </c>
       <c r="H37"/>
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
@@ -1948,6 +1980,114 @@
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
       <c r="L41" s="7"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C42" s="17"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="7"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C43" s="17"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="7"/>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C44" s="17"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="7"/>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C45" s="17"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="7"/>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C46" s="17"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="7"/>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C47" s="17"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="7"/>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C48" s="17"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="7"/>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C49" s="17"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="7"/>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C50" s="17"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="7"/>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C51" s="17"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="7"/>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C52" s="17"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="7"/>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C53" s="17"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
McCarter & Ash Reading Test 2 Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351D9D61-9ADD-4308-AA32-01AA047C3160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9230D65B-742A-4EB2-B8CD-35694931D528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>McCarter&amp;Ash Test 1</t>
+  </si>
+  <si>
+    <t>McCarter&amp;Ash Test 2</t>
   </si>
 </sst>
 </file>
@@ -768,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,12 +851,10 @@
         <v>4.5</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="9">
-        <v>5</v>
-      </c>
+      <c r="K4" s="9"/>
       <c r="L4" s="7">
         <f t="shared" ref="L4:L17" si="0">(G4+I4+J4+K4)/4</f>
-        <v>3.875</v>
+        <v>2.625</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -876,12 +877,10 @@
       <c r="H5"/>
       <c r="I5" s="8"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="9">
-        <v>5</v>
-      </c>
+      <c r="K5" s="9"/>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>2.625</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -971,12 +970,10 @@
       <c r="J8" s="9">
         <v>4.5</v>
       </c>
-      <c r="K8" s="9">
-        <v>5</v>
-      </c>
+      <c r="K8" s="9"/>
       <c r="L8" s="7">
         <f t="shared" si="0"/>
-        <v>2.375</v>
+        <v>1.125</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -999,12 +996,10 @@
         <v>6</v>
       </c>
       <c r="J9" s="9"/>
-      <c r="K9" s="9">
-        <v>5</v>
-      </c>
+      <c r="K9" s="9"/>
       <c r="L9" s="7">
         <f t="shared" si="0"/>
-        <v>2.75</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1032,12 +1027,10 @@
         <v>5.5</v>
       </c>
       <c r="J10" s="9"/>
-      <c r="K10" s="9">
-        <v>5</v>
-      </c>
+      <c r="K10" s="9"/>
       <c r="L10" s="7">
         <f t="shared" si="0"/>
-        <v>4.375</v>
+        <v>3.125</v>
       </c>
       <c r="N10" s="7"/>
     </row>
@@ -1058,12 +1051,10 @@
       <c r="J11" s="9">
         <v>6</v>
       </c>
-      <c r="K11" s="9">
-        <v>5</v>
-      </c>
+      <c r="K11" s="9"/>
       <c r="L11" s="7">
         <f>(G11+I11+J11+K11)/4</f>
-        <v>2.75</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1083,12 +1074,10 @@
       <c r="J12" s="9">
         <v>4</v>
       </c>
-      <c r="K12" s="9">
-        <v>5</v>
-      </c>
+      <c r="K12" s="9"/>
       <c r="L12" s="7">
         <f>(G12+I12+J12+K12)/4</f>
-        <v>2.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1111,9 +1100,7 @@
         <v>6</v>
       </c>
       <c r="J13" s="9"/>
-      <c r="K13" s="9">
-        <v>5</v>
-      </c>
+      <c r="K13" s="9"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1561,12 +1548,10 @@
         <v>6.5</v>
       </c>
       <c r="J26" s="11"/>
-      <c r="K26" s="9">
-        <v>5</v>
-      </c>
+      <c r="K26" s="9"/>
       <c r="L26" s="7">
         <f t="shared" si="2"/>
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="27" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1942,11 +1927,25 @@
       <c r="K37" s="11"/>
       <c r="L37" s="7"/>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="13">
+        <v>35</v>
+      </c>
+      <c r="D38" s="14">
+        <v>45520</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
       <c r="F38" s="6"/>
       <c r="G38" s="10"/>
-      <c r="H38"/>
-      <c r="I38" s="10"/>
+      <c r="H38">
+        <v>25</v>
+      </c>
+      <c r="I38" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6</v>
+      </c>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
       <c r="L38" s="7"/>

</xml_diff>

<commit_message>
McCarter & Ash Reading Test 3 Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9230D65B-742A-4EB2-B8CD-35694931D528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8784A959-24F7-43D6-BAD1-A3247510654D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>McCarter&amp;Ash Test 2</t>
+  </si>
+  <si>
+    <t>McCarter&amp;Ash Test 3</t>
+  </si>
+  <si>
+    <t>IELTS_Ready_</t>
   </si>
 </sst>
 </file>
@@ -771,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1950,16 +1956,39 @@
       <c r="K38" s="11"/>
       <c r="L38" s="7"/>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C39" s="13">
+        <v>36</v>
+      </c>
+      <c r="D39" s="14">
+        <v>45522</v>
+      </c>
+      <c r="E39" t="s">
+        <v>46</v>
+      </c>
       <c r="F39" s="6"/>
-      <c r="G39" s="10"/>
-      <c r="H39"/>
-      <c r="I39" s="10"/>
+      <c r="G39" s="8"/>
+      <c r="H39">
+        <v>25</v>
+      </c>
+      <c r="I39" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6</v>
+      </c>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
       <c r="L39" s="7"/>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C40" s="13">
+        <v>37</v>
+      </c>
+      <c r="D40" s="14">
+        <v>45522</v>
+      </c>
+      <c r="E40" t="s">
+        <v>47</v>
+      </c>
       <c r="F40" s="6"/>
       <c r="G40" s="10"/>
       <c r="H40"/>

</xml_diff>

<commit_message>
IELTS READY Mock Test 1; Listening and Reading Done.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8784A959-24F7-43D6-BAD1-A3247510654D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823AB04D-0CC6-46E3-955F-03BA8E9CC938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
     <t>McCarter&amp;Ash Test 3</t>
   </si>
   <si>
-    <t>IELTS_Ready_</t>
+    <t>IELTS_Ready_MockTest_1</t>
   </si>
 </sst>
 </file>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -787,7 +787,7 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="6.54296875" style="13" customWidth="1"/>
     <col min="4" max="4" width="12.90625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="24.6328125" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="6.54296875" customWidth="1"/>
     <col min="8" max="8" width="10.1796875" style="7" customWidth="1"/>
@@ -1944,7 +1944,7 @@
         <v>45</v>
       </c>
       <c r="F38" s="6"/>
-      <c r="G38" s="10"/>
+      <c r="G38" s="8"/>
       <c r="H38">
         <v>25</v>
       </c>
@@ -1979,7 +1979,7 @@
       <c r="K39" s="11"/>
       <c r="L39" s="7"/>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C40" s="13">
         <v>37</v>
       </c>
@@ -1989,10 +1989,20 @@
       <c r="E40" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="10"/>
-      <c r="H40"/>
-      <c r="I40" s="10"/>
+      <c r="F40" s="6">
+        <v>31</v>
+      </c>
+      <c r="G40" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>29</v>
+      </c>
+      <c r="I40" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
       <c r="J40" s="11"/>
       <c r="K40" s="11"/>
       <c r="L40" s="7"/>

</xml_diff>

<commit_message>
Practiced IELTS Ready MockTest 3 Reading.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823AB04D-0CC6-46E3-955F-03BA8E9CC938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8654CA51-B715-4CBD-A170-298B6FDEABAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>IELTS_Ready_MockTest_1</t>
+  </si>
+  <si>
+    <t>IELTS_Ready_MockTest_2</t>
+  </si>
+  <si>
+    <t>IELTS_Ready_MockTest_3</t>
   </si>
 </sst>
 </file>
@@ -777,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2007,19 +2013,53 @@
       <c r="K40" s="11"/>
       <c r="L40" s="7"/>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="F41" s="6"/>
-      <c r="G41" s="10"/>
-      <c r="H41"/>
-      <c r="I41" s="10"/>
+    <row r="41" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C41" s="13">
+        <v>38</v>
+      </c>
+      <c r="D41" s="14">
+        <v>45522</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="6">
+        <v>29</v>
+      </c>
+      <c r="G41" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
+      <c r="H41">
+        <v>26</v>
+      </c>
+      <c r="I41" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6</v>
+      </c>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
       <c r="L41" s="7"/>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C42" s="13">
+        <v>39</v>
+      </c>
+      <c r="D42" s="14">
+        <v>45525</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
       <c r="F42" s="6"/>
-      <c r="G42" s="10"/>
-      <c r="I42" s="10"/>
+      <c r="G42" s="8"/>
+      <c r="H42">
+        <v>31</v>
+      </c>
+      <c r="I42" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
       <c r="L42" s="7"/>

</xml_diff>

<commit_message>
Cambridge 16 Test1 Listening & Reading Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE729EC-CA22-48D6-A254-0D4C134C0752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C638BC89-8F7E-4A91-8BFC-D4FC67C180A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>IELTS_Ready_MockTest_3</t>
+  </si>
+  <si>
+    <t>IELTS16_Test1</t>
   </si>
 </sst>
 </file>
@@ -283,7 +286,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,6 +322,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -326,7 +330,26 @@
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="center"/>
@@ -383,22 +406,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -425,23 +432,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L53" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="C3:L53" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L56" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="C3:L56" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
   <tableColumns count="10">
-    <tableColumn id="10" xr3:uid="{5AC48ABC-B60E-45DE-9969-4F077A234137}" name="No." dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{5AC48ABC-B60E-45DE-9969-4F077A234137}" name="No." dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{DC71C96E-388E-4427-9265-6CF875C8C5D7}" name="Course"/>
-    <tableColumn id="9" xr3:uid="{D3F721AC-61B7-43CC-AF2E-6E0AC12EB3B2}" name="Lis_Mark" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A705CE31-7A52-4C7A-85F3-5408CE0B0560}" name="Listening" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{D3F721AC-61B7-43CC-AF2E-6E0AC12EB3B2}" name="Lis_Mark" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{A705CE31-7A52-4C7A-85F3-5408CE0B0560}" name="Listening" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Lis_Mark]],Table3[[From]:[To]], 3, TRUE),"No Grade")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{65004197-C26E-4874-9A2E-3A56EC978737}" name="Read_Mark"/>
-    <tableColumn id="4" xr3:uid="{EF57AC4F-0BC5-47DA-A549-5E18B8D107B5}" name="Reading" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{65004197-C26E-4874-9A2E-3A56EC978737}" name="Read_Mark" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{EF57AC4F-0BC5-47DA-A549-5E18B8D107B5}" name="Reading" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15AFFB2A-07B5-47FC-9437-545D8A8916B1}" name="Writing" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{C0566DD1-3113-4CF0-96DC-1B3F892D0FAF}" name="Speaking" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{5E672D08-F03A-4519-AD28-B657B411A22F}" name="Overall" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{15AFFB2A-07B5-47FC-9437-545D8A8916B1}" name="Writing" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C0566DD1-3113-4CF0-96DC-1B3F892D0FAF}" name="Speaking" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{5E672D08-F03A-4519-AD28-B657B411A22F}" name="Overall" dataDxfId="8">
       <calculatedColumnFormula>(G4+I4+J4+K4)/4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -450,15 +457,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}" name="Table3" displayName="Table3" ref="D4:F20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}" name="Table3" displayName="Table3" ref="D4:F20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="D4:F20" xr:uid="{7DB38F47-88FD-45C7-A867-5DD4AE94A29A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:F20">
     <sortCondition ref="F4:F20"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2FE19739-2635-4933-9D55-4983D35E031D}" name="From" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A722DE31-0502-40CE-AE01-B2178E5F2D6E}" name="To" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{8081C4D8-49F2-41DD-A868-2F4234154D0E}" name="Band_Score" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2FE19739-2635-4933-9D55-4983D35E031D}" name="From" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A722DE31-0502-40CE-AE01-B2178E5F2D6E}" name="To" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{8081C4D8-49F2-41DD-A868-2F4234154D0E}" name="Band_Score" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -781,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N53"/>
+  <dimension ref="B1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -855,7 +862,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="17">
         <v>13</v>
       </c>
       <c r="I4" s="8">
@@ -886,7 +893,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>5.5</v>
       </c>
-      <c r="H5"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="8"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -912,7 +919,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="17">
         <v>20</v>
       </c>
       <c r="I6" s="8">
@@ -947,7 +954,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="17">
         <v>20</v>
       </c>
       <c r="I7" s="8">
@@ -977,7 +984,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="8"/>
-      <c r="H8"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9">
         <v>4.5</v>
@@ -1000,7 +1007,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="8"/>
-      <c r="H9">
+      <c r="H9" s="17">
         <v>24</v>
       </c>
       <c r="I9" s="8">
@@ -1031,7 +1038,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="17">
         <v>20</v>
       </c>
       <c r="I10" s="8">
@@ -1058,7 +1065,7 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="8"/>
-      <c r="H11"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="8"/>
       <c r="J11" s="9">
         <v>6</v>
@@ -1081,7 +1088,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="8"/>
-      <c r="H12"/>
+      <c r="H12" s="17"/>
       <c r="I12" s="8"/>
       <c r="J12" s="9">
         <v>4</v>
@@ -1104,7 +1111,7 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="8"/>
-      <c r="H13">
+      <c r="H13" s="17">
         <v>25</v>
       </c>
       <c r="I13" s="8">
@@ -1132,7 +1139,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="17">
         <v>28</v>
       </c>
       <c r="I14" s="8">
@@ -1167,7 +1174,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="17">
         <v>29</v>
       </c>
       <c r="I15" s="8">
@@ -1202,7 +1209,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="17">
         <v>26</v>
       </c>
       <c r="I16" s="8">
@@ -1237,7 +1244,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="17">
         <v>32</v>
       </c>
       <c r="I17" s="8">
@@ -1272,7 +1279,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="17">
         <v>24</v>
       </c>
       <c r="I18" s="8">
@@ -1307,7 +1314,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="17">
         <v>25</v>
       </c>
       <c r="I19" s="8">
@@ -1342,7 +1349,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="17">
         <v>26</v>
       </c>
       <c r="I20" s="8">
@@ -1377,7 +1384,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="17">
         <v>29</v>
       </c>
       <c r="I21" s="8">
@@ -1412,7 +1419,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="17">
         <v>22</v>
       </c>
       <c r="I22" s="8">
@@ -1447,7 +1454,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="17">
         <v>25</v>
       </c>
       <c r="I23" s="8">
@@ -1482,7 +1489,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="17">
         <v>34</v>
       </c>
       <c r="I24" s="8">
@@ -1496,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="7">
-        <f t="shared" ref="L24:L36" si="2">(G24+I24+J24+K24)/4</f>
+        <f t="shared" ref="L24:L43" si="2">(G24+I24+J24+K24)/4</f>
         <v>6.5</v>
       </c>
     </row>
@@ -1517,7 +1524,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>8</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="17">
         <v>32</v>
       </c>
       <c r="I25" s="8">
@@ -1552,7 +1559,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="17">
         <v>27</v>
       </c>
       <c r="I26" s="8">
@@ -1583,7 +1590,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="17">
         <v>24</v>
       </c>
       <c r="I27" s="8">
@@ -1618,7 +1625,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="17">
         <v>32</v>
       </c>
       <c r="I28" s="8">
@@ -1653,7 +1660,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="17">
         <v>32</v>
       </c>
       <c r="I29" s="8">
@@ -1688,7 +1695,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>8</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="17">
         <v>32</v>
       </c>
       <c r="I30" s="8">
@@ -1723,7 +1730,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>9</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="17">
         <v>27</v>
       </c>
       <c r="I31" s="8">
@@ -1758,7 +1765,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="17">
         <v>29</v>
       </c>
       <c r="I32" s="8">
@@ -1793,7 +1800,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7.5</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="17">
         <v>33</v>
       </c>
       <c r="I33" s="8">
@@ -1828,7 +1835,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>8</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="17">
         <v>30</v>
       </c>
       <c r="I34" s="8">
@@ -1863,7 +1870,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="17">
         <v>34</v>
       </c>
       <c r="I35" s="8">
@@ -1898,7 +1905,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="17">
         <v>27</v>
       </c>
       <c r="I36" s="8">
@@ -1928,7 +1935,7 @@
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="8"/>
-      <c r="H37">
+      <c r="H37" s="17">
         <v>24</v>
       </c>
       <c r="I37" s="8">
@@ -1937,7 +1944,10 @@
       </c>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
-      <c r="L37" s="7"/>
+      <c r="L37" s="7">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="38" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="13">
@@ -1951,7 +1961,7 @@
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="8"/>
-      <c r="H38">
+      <c r="H38" s="17">
         <v>25</v>
       </c>
       <c r="I38" s="8">
@@ -1960,7 +1970,10 @@
       </c>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
-      <c r="L38" s="7"/>
+      <c r="L38" s="7">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="39" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C39" s="13">
@@ -1974,7 +1987,7 @@
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="8"/>
-      <c r="H39">
+      <c r="H39" s="17">
         <v>25</v>
       </c>
       <c r="I39" s="8">
@@ -1983,7 +1996,10 @@
       </c>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
-      <c r="L39" s="7"/>
+      <c r="L39" s="7">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="40" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C40" s="13">
@@ -2002,7 +2018,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>7</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="17">
         <v>29</v>
       </c>
       <c r="I40" s="8">
@@ -2011,7 +2027,10 @@
       </c>
       <c r="J40" s="11"/>
       <c r="K40" s="11"/>
-      <c r="L40" s="7"/>
+      <c r="L40" s="7">
+        <f t="shared" si="2"/>
+        <v>3.375</v>
+      </c>
     </row>
     <row r="41" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C41" s="13">
@@ -2030,7 +2049,7 @@
         <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
         <v>6.5</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="17">
         <v>26</v>
       </c>
       <c r="I41" s="8">
@@ -2039,7 +2058,10 @@
       </c>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
-      <c r="L41" s="7"/>
+      <c r="L41" s="7">
+        <f t="shared" si="2"/>
+        <v>3.125</v>
+      </c>
     </row>
     <row r="42" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C42" s="13">
@@ -2053,7 +2075,7 @@
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="8"/>
-      <c r="H42">
+      <c r="H42" s="17">
         <v>31</v>
       </c>
       <c r="I42" s="8">
@@ -2062,19 +2084,46 @@
       </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
-      <c r="L42" s="7"/>
-    </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="F43" s="6"/>
-      <c r="G43" s="10"/>
-      <c r="I43" s="10"/>
+      <c r="L42" s="7">
+        <f t="shared" si="2"/>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C43" s="13">
+        <v>40</v>
+      </c>
+      <c r="D43" s="14">
+        <v>45527</v>
+      </c>
+      <c r="E43" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="6">
+        <v>35</v>
+      </c>
+      <c r="G43" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
+      <c r="H43" s="17">
+        <v>32</v>
+      </c>
+      <c r="I43" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
-      <c r="L43" s="7"/>
+      <c r="L43" s="7">
+        <f t="shared" si="2"/>
+        <v>3.75</v>
+      </c>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F44" s="6"/>
       <c r="G44" s="10"/>
+      <c r="H44" s="17"/>
       <c r="I44" s="10"/>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
@@ -2083,6 +2132,7 @@
     <row r="45" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F45" s="6"/>
       <c r="G45" s="10"/>
+      <c r="H45" s="17"/>
       <c r="I45" s="10"/>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
@@ -2091,6 +2141,7 @@
     <row r="46" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F46" s="6"/>
       <c r="G46" s="10"/>
+      <c r="H46" s="17"/>
       <c r="I46" s="10"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
@@ -2099,6 +2150,7 @@
     <row r="47" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F47" s="6"/>
       <c r="G47" s="10"/>
+      <c r="H47" s="17"/>
       <c r="I47" s="10"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
@@ -2107,6 +2159,7 @@
     <row r="48" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F48" s="6"/>
       <c r="G48" s="10"/>
+      <c r="H48" s="17"/>
       <c r="I48" s="10"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
@@ -2115,6 +2168,7 @@
     <row r="49" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F49" s="6"/>
       <c r="G49" s="10"/>
+      <c r="H49" s="17"/>
       <c r="I49" s="10"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
@@ -2123,6 +2177,7 @@
     <row r="50" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F50" s="6"/>
       <c r="G50" s="10"/>
+      <c r="H50" s="17"/>
       <c r="I50" s="10"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
@@ -2131,6 +2186,7 @@
     <row r="51" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F51" s="6"/>
       <c r="G51" s="10"/>
+      <c r="H51" s="17"/>
       <c r="I51" s="10"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
@@ -2139,6 +2195,7 @@
     <row r="52" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F52" s="6"/>
       <c r="G52" s="10"/>
+      <c r="H52" s="17"/>
       <c r="I52" s="10"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
@@ -2147,10 +2204,38 @@
     <row r="53" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F53" s="6"/>
       <c r="G53" s="10"/>
+      <c r="H53" s="17"/>
       <c r="I53" s="10"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
       <c r="L53" s="7"/>
+    </row>
+    <row r="54" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F54" s="6"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="7"/>
+    </row>
+    <row r="55" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F55" s="6"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="7"/>
+    </row>
+    <row r="56" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F56" s="6"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Official IELTS Practice Material 2 Practiced.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDF8477-38C0-4FC2-83DF-48D580E635CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19262EB7-B7D4-4FAB-B6B9-86B87D3F6467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>IELTS_Ready_MockTest_5</t>
+  </si>
+  <si>
+    <t>Official IELTS Practice material 2</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
   <dimension ref="B1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,7 +808,7 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="6.54296875" style="13" customWidth="1"/>
     <col min="4" max="4" width="12.90625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="24.6328125" customWidth="1"/>
+    <col min="5" max="5" width="27.36328125" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="6.54296875" customWidth="1"/>
     <col min="8" max="8" width="10.1796875" style="7" customWidth="1"/>
@@ -2193,18 +2196,44 @@
         <v>4</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" ref="L45" si="3">(G45+I45+J45+K45)/4</f>
+        <f t="shared" ref="L45:L46" si="3">(G45+I45+J45+K45)/4</f>
         <v>5.75</v>
       </c>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="F46" s="6"/>
-      <c r="G46" s="10"/>
-      <c r="H46"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="7"/>
+    <row r="46" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C46" s="13">
+        <v>42</v>
+      </c>
+      <c r="D46" s="14">
+        <v>45530</v>
+      </c>
+      <c r="E46" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="6">
+        <v>31</v>
+      </c>
+      <c r="G46" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="H46">
+        <v>31</v>
+      </c>
+      <c r="I46" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="J46" s="11">
+        <v>6</v>
+      </c>
+      <c r="K46" s="11">
+        <v>4</v>
+      </c>
+      <c r="L46" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F47" s="6"/>

</xml_diff>

<commit_message>
Practiced Cambridge 19 Test1.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19262EB7-B7D4-4FAB-B6B9-86B87D3F6467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87511B4E-20EC-4F91-BBF3-52133E3341C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Official IELTS Practice material 2</t>
+  </si>
+  <si>
+    <t>IELTS19_Test1</t>
   </si>
 </sst>
 </file>
@@ -799,7 +802,7 @@
   <dimension ref="B1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2196,7 +2199,7 @@
         <v>4</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" ref="L45:L46" si="3">(G45+I45+J45+K45)/4</f>
+        <f t="shared" ref="L45:L47" si="3">(G45+I45+J45+K45)/4</f>
         <v>5.75</v>
       </c>
     </row>
@@ -2235,14 +2238,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="F47" s="6"/>
-      <c r="G47" s="10"/>
-      <c r="H47"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="7"/>
+    <row r="47" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C47" s="13">
+        <v>43</v>
+      </c>
+      <c r="D47" s="14">
+        <v>45531</v>
+      </c>
+      <c r="E47" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="6">
+        <v>30</v>
+      </c>
+      <c r="G47" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="H47">
+        <v>35</v>
+      </c>
+      <c r="I47" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
+      <c r="J47" s="11">
+        <v>6</v>
+      </c>
+      <c r="K47" s="11">
+        <v>4</v>
+      </c>
+      <c r="L47" s="7">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F48" s="6"/>

</xml_diff>

<commit_message>
Practiced Cambridge 19 Test2.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87511B4E-20EC-4F91-BBF3-52133E3341C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E6D1F4-79B9-4998-9F8B-CCDA7E58CA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>IELTS19_Test1</t>
+  </si>
+  <si>
+    <t>IELTS19_Test2</t>
   </si>
 </sst>
 </file>
@@ -802,7 +805,7 @@
   <dimension ref="B1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="N49" sqref="N49"/>
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2199,7 +2202,7 @@
         <v>4</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" ref="L45:L47" si="3">(G45+I45+J45+K45)/4</f>
+        <f t="shared" ref="L45:L48" si="3">(G45+I45+J45+K45)/4</f>
         <v>5.75</v>
       </c>
     </row>
@@ -2273,14 +2276,40 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="F48" s="6"/>
-      <c r="G48" s="10"/>
-      <c r="H48"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="7"/>
+    <row r="48" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C48" s="13">
+        <v>44</v>
+      </c>
+      <c r="D48" s="14">
+        <v>45532</v>
+      </c>
+      <c r="E48" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="6">
+        <v>36</v>
+      </c>
+      <c r="G48" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
+      <c r="H48">
+        <v>35</v>
+      </c>
+      <c r="I48" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
+      <c r="J48" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="K48" s="11">
+        <v>4</v>
+      </c>
+      <c r="L48" s="7">
+        <f t="shared" si="3"/>
+        <v>6.625</v>
+      </c>
     </row>
     <row r="49" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F49" s="6"/>

</xml_diff>

<commit_message>
Practice Cambridge 19 Test 3.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E6D1F4-79B9-4998-9F8B-CCDA7E58CA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DBF236-93FA-49D2-8668-849AD6CF334F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>IELTS19_Test2</t>
+  </si>
+  <si>
+    <t>IELTS19_Test3</t>
+  </si>
+  <si>
+    <t>The IELTS EXAM DAY</t>
   </si>
 </sst>
 </file>
@@ -204,7 +210,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +248,13 @@
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -301,7 +314,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,12 +344,22 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -804,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2202,7 +2225,7 @@
         <v>4</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" ref="L45:L48" si="3">(G45+I45+J45+K45)/4</f>
+        <f t="shared" ref="L45:L49" si="3">(G45+I45+J45+K45)/4</f>
         <v>5.75</v>
       </c>
     </row>
@@ -2311,16 +2334,48 @@
         <v>6.625</v>
       </c>
     </row>
-    <row r="49" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F49" s="6"/>
-      <c r="G49" s="10"/>
-      <c r="H49"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="7"/>
-    </row>
-    <row r="50" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C49" s="13">
+        <v>45</v>
+      </c>
+      <c r="D49" s="14">
+        <v>45533</v>
+      </c>
+      <c r="E49" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" s="6">
+        <v>34</v>
+      </c>
+      <c r="G49" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7.5</v>
+      </c>
+      <c r="H49">
+        <v>36</v>
+      </c>
+      <c r="I49" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
+      <c r="J49" s="11">
+        <v>6</v>
+      </c>
+      <c r="K49" s="11">
+        <v>4</v>
+      </c>
+      <c r="L49" s="7">
+        <f t="shared" si="3"/>
+        <v>6.375</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C50" s="13">
+        <v>45</v>
+      </c>
+      <c r="D50" s="14">
+        <v>45534</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="10"/>
       <c r="H50"/>
@@ -2329,7 +2384,13 @@
       <c r="K50" s="11"/>
       <c r="L50" s="7"/>
     </row>
-    <row r="51" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C51" s="13">
+        <v>45</v>
+      </c>
+      <c r="D51" s="14">
+        <v>45535</v>
+      </c>
       <c r="F51" s="6"/>
       <c r="G51" s="10"/>
       <c r="H51"/>
@@ -2338,7 +2399,13 @@
       <c r="K51" s="11"/>
       <c r="L51" s="7"/>
     </row>
-    <row r="52" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C52" s="13">
+        <v>45</v>
+      </c>
+      <c r="D52" s="14">
+        <v>45536</v>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="10"/>
       <c r="H52"/>
@@ -2347,7 +2414,13 @@
       <c r="K52" s="11"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C53" s="13">
+        <v>45</v>
+      </c>
+      <c r="D53" s="14">
+        <v>45537</v>
+      </c>
       <c r="F53" s="6"/>
       <c r="G53" s="10"/>
       <c r="H53"/>
@@ -2356,7 +2429,13 @@
       <c r="K53" s="11"/>
       <c r="L53" s="7"/>
     </row>
-    <row r="54" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C54" s="13">
+        <v>45</v>
+      </c>
+      <c r="D54" s="14">
+        <v>45538</v>
+      </c>
       <c r="F54" s="6"/>
       <c r="G54" s="10"/>
       <c r="H54"/>
@@ -2365,16 +2444,26 @@
       <c r="K54" s="11"/>
       <c r="L54" s="7"/>
     </row>
-    <row r="55" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F55" s="6"/>
-      <c r="G55" s="10"/>
-      <c r="H55"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="7"/>
-    </row>
-    <row r="56" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C55" s="15">
+        <v>45</v>
+      </c>
+      <c r="D55" s="18">
+        <v>45539</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F55" s="20"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="21"/>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D56" s="14"/>
       <c r="F56" s="6"/>
       <c r="G56" s="10"/>
       <c r="H56"/>
@@ -2408,17 +2497,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Practiced Premium Mock Test 2.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF59C4-E274-4D1B-9670-4EBA9F1D4AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1812162A-80D9-4FB9-9725-F5E549AE0A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Computer_Friendly_Test</t>
+  </si>
+  <si>
+    <t>IELTS_Premium_MockTest2</t>
+  </si>
+  <si>
+    <t>Cambridge19_Test4</t>
   </si>
 </sst>
 </file>
@@ -320,7 +326,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -366,10 +372,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -479,8 +481,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L56" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="C3:L56" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}" name="Table1" displayName="Table1" ref="C3:L62" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="C3:L62" xr:uid="{7D616C37-89EF-4EB9-8697-F85C377504D8}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{5AC48ABC-B60E-45DE-9969-4F077A234137}" name="No." dataDxfId="13"/>
     <tableColumn id="1" xr3:uid="{ACB8A356-FC94-4E61-904C-F3C2DEEB68FC}" name="Date" dataDxfId="12"/>
@@ -835,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N56"/>
+  <dimension ref="B1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2397,12 +2399,12 @@
         <v>6.5</v>
       </c>
       <c r="H50"/>
-      <c r="I50" s="10"/>
+      <c r="I50" s="8"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
       <c r="L50" s="7"/>
     </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="13">
         <v>46</v>
       </c>
@@ -2413,51 +2415,79 @@
         <v>59</v>
       </c>
       <c r="F51" s="6"/>
-      <c r="G51" s="10"/>
+      <c r="G51" s="8"/>
       <c r="H51"/>
-      <c r="I51" s="10"/>
+      <c r="I51" s="8"/>
       <c r="J51" s="11">
         <v>6</v>
       </c>
       <c r="K51" s="11"/>
       <c r="L51" s="7"/>
     </row>
-    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C52" s="23">
+    <row r="52" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C52" s="13">
         <v>45</v>
       </c>
       <c r="D52" s="14">
         <v>45535</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="10"/>
-      <c r="H52"/>
-      <c r="I52" s="10"/>
+      <c r="E52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F52" s="6">
+        <v>32</v>
+      </c>
+      <c r="G52" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="H52">
+        <v>28</v>
+      </c>
+      <c r="I52" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C53" s="23">
-        <v>45</v>
+    <row r="53" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C53" s="13">
+        <v>46</v>
       </c>
       <c r="D53" s="14">
-        <v>45536</v>
-      </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="10"/>
-      <c r="H53"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="11"/>
+        <v>45535</v>
+      </c>
+      <c r="E53" t="s">
+        <v>61</v>
+      </c>
+      <c r="F53" s="6">
+        <v>29</v>
+      </c>
+      <c r="G53" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>6.5</v>
+      </c>
+      <c r="H53">
+        <v>32</v>
+      </c>
+      <c r="I53" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>7</v>
+      </c>
+      <c r="J53" s="11">
+        <v>6</v>
+      </c>
       <c r="K53" s="11"/>
       <c r="L53" s="7"/>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C54" s="23">
+      <c r="C54" s="13">
         <v>45</v>
       </c>
       <c r="D54" s="14">
-        <v>45537</v>
+        <v>45536</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="10"/>
@@ -2468,37 +2498,97 @@
       <c r="L54" s="7"/>
     </row>
     <row r="55" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C55" s="23">
+      <c r="C55" s="13">
         <v>45</v>
       </c>
       <c r="D55" s="14">
-        <v>45538</v>
+        <v>45537</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="10"/>
-      <c r="H55" s="24"/>
+      <c r="H55"/>
       <c r="I55" s="10"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
       <c r="L55" s="7"/>
     </row>
     <row r="56" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C56" s="15">
+      <c r="C56" s="13">
         <v>45</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D56" s="14">
+        <v>45538</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="10"/>
+      <c r="H56"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="7"/>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C57" s="15">
+        <v>45</v>
+      </c>
+      <c r="D57" s="16">
         <v>45539</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E57" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F56" s="18"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="19"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="19"/>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="F58" s="6"/>
+      <c r="G58" s="10"/>
+      <c r="H58"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="7"/>
+    </row>
+    <row r="59" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="F59" s="6"/>
+      <c r="G59" s="10"/>
+      <c r="H59"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="7"/>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="F60" s="6"/>
+      <c r="G60" s="10"/>
+      <c r="H60"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="7"/>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="F61" s="6"/>
+      <c r="G61" s="10"/>
+      <c r="H61"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="7"/>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="F62" s="6"/>
+      <c r="G62" s="10"/>
+      <c r="H62"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Practiced IELTS 19 Test 4.
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1812162A-80D9-4FB9-9725-F5E549AE0A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493AE398-11BC-4E7A-A8DF-993F6D484FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,7 +840,7 @@
   <dimension ref="B1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Practiced Cambridge 16 Test 3!
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F75061D-E3F6-47AF-8559-1224D54577C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61608F02-45E8-4FF8-B318-E675708801D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Cambridge16_Test3</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -344,7 +347,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,9 +375,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -858,7 +858,7 @@
   <dimension ref="B1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2255,7 +2255,7 @@
         <v>4</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" ref="L45:L58" si="3">(G45+I45+J45+K45)/4</f>
+        <f t="shared" ref="L45:L59" si="3">(G45+I45+J45+K45)/4</f>
         <v>5.75</v>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C59" s="13">
         <v>46</v>
       </c>
@@ -2659,21 +2659,33 @@
       <c r="E59" t="s">
         <v>67</v>
       </c>
-      <c r="F59" s="6"/>
-      <c r="G59" s="10"/>
-      <c r="H59"/>
-      <c r="I59" s="10"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="7"/>
+      <c r="F59" s="6">
+        <v>35</v>
+      </c>
+      <c r="G59" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Lis_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8</v>
+      </c>
+      <c r="H59">
+        <v>37</v>
+      </c>
+      <c r="I59" s="8">
+        <f>IFERROR(INDEX(Sheet2!$F$5:$F$20, MATCH(Table1[[#This Row],[Read_Mark]], Sheet2!$D$5:$D$20, 1)),"No Grade")</f>
+        <v>8.5</v>
+      </c>
+      <c r="J59" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="K59" s="11">
+        <v>5</v>
+      </c>
+      <c r="L59" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="60" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C60" s="13">
-        <v>47</v>
-      </c>
-      <c r="D60" s="14">
-        <v>45538</v>
-      </c>
+      <c r="D60" s="14"/>
       <c r="F60" s="6"/>
       <c r="G60" s="10"/>
       <c r="H60"/>
@@ -2683,22 +2695,22 @@
       <c r="L60" s="7"/>
     </row>
     <row r="61" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C61" s="15">
-        <v>45</v>
-      </c>
-      <c r="D61" s="16">
+      <c r="C61" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="15">
         <v>45539</v>
       </c>
-      <c r="E61" s="20" t="s">
+      <c r="E61" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F61" s="18"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="19"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="18"/>
     </row>
     <row r="62" spans="3:12" x14ac:dyDescent="0.35">
       <c r="F62" s="6"/>
@@ -2734,17 +2746,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Harvested what we've grown, an overall 7.5. HEHEHE
</commit_message>
<xml_diff>
--- a/my_IELTS_Scores.xlsx
+++ b/my_IELTS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF990D0-34B1-44C6-B375-5CCF6A2FB680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6971BC-977F-4355-99F1-C74589D891DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,7 +246,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +286,17 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Aptos Narrow"/>
@@ -380,19 +391,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -860,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="Q59" sqref="Q59"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2258,7 +2271,7 @@
         <v>4</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" ref="L45:L59" si="3">(G45+I45+J45+K45)/4</f>
+        <f t="shared" ref="L45:L61" si="3">(G45+I45+J45+K45)/4</f>
         <v>5.75</v>
       </c>
     </row>
@@ -2735,22 +2748,32 @@
       <c r="L60" s="7"/>
     </row>
     <row r="61" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D61" s="15">
+      <c r="D61" s="18">
         <v>45539</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F61" s="17"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="16"/>
-      <c r="L61" s="18"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="21">
+        <v>8</v>
+      </c>
+      <c r="H61" s="19"/>
+      <c r="I61" s="21">
+        <v>8</v>
+      </c>
+      <c r="J61" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="K61" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="L61" s="21">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="62" spans="3:15" x14ac:dyDescent="0.35">
       <c r="F62" s="6"/>
@@ -2786,17 +2809,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.35">

</xml_diff>